<commit_message>
ISAICP-2973: Fix 'field_is_logo'. Allow also new images.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="354">
   <si>
     <t>Work in progress</t>
   </si>
@@ -1092,6 +1092,9 @@
   </si>
   <si>
     <t>Eurovoc</t>
+  </si>
+  <si>
+    <t>acme.jpg</t>
   </si>
 </sst>
 </file>
@@ -1402,6 +1405,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1426,12 +1435,6 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -2132,37 +2135,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="63" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="64" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="68" t="s">
         <v>220</v>
       </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="66"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="70"/>
       <c r="P1" s="57"/>
-      <c r="Q1" s="62" t="s">
+      <c r="Q1" s="66" t="s">
         <v>219</v>
       </c>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
     </row>
     <row r="2" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="56" t="s">
@@ -2553,7 +2556,9 @@
       <c r="I7" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="J7" s="29"/>
+      <c r="J7" s="46" t="s">
+        <v>353</v>
+      </c>
       <c r="K7" s="29" t="s">
         <v>222</v>
       </c>
@@ -9059,7 +9064,7 @@
       <c r="Q109" s="44">
         <v>41977</v>
       </c>
-      <c r="R109" s="67">
+      <c r="R109" s="59">
         <v>4463</v>
       </c>
       <c r="S109" s="7">
@@ -9210,7 +9215,7 @@
       <c r="A112" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B112" s="68">
+      <c r="B112" s="60">
         <v>59183</v>
       </c>
       <c r="C112" s="13" t="s">
@@ -9515,7 +9520,7 @@
       <c r="A117" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B117" s="68">
+      <c r="B117" s="60">
         <v>59228</v>
       </c>
       <c r="C117" s="13" t="s">
@@ -9820,7 +9825,7 @@
       <c r="A122" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B122" s="68">
+      <c r="B122" s="60">
         <v>59264</v>
       </c>
       <c r="C122" s="13" t="s">
@@ -9881,7 +9886,7 @@
       <c r="A123" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B123" s="69">
+      <c r="B123" s="61">
         <v>59271</v>
       </c>
       <c r="C123" s="13" t="s">
@@ -11137,7 +11142,7 @@
       <c r="S143" s="37">
         <v>0</v>
       </c>
-      <c r="T143" s="70">
+      <c r="T143" s="62">
         <v>2</v>
       </c>
       <c r="U143" s="28" t="s">
@@ -11564,7 +11569,7 @@
       <c r="S150" s="37">
         <v>0</v>
       </c>
-      <c r="T150" s="70">
+      <c r="T150" s="62">
         <v>11</v>
       </c>
       <c r="U150" s="28" t="s">

</xml_diff>

<commit_message>
ISAICP-3230: Add tests for 'prepare' migration.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$2:$V$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$2:$V$13</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>No</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Migrate</t>
   </si>
   <si>
-    <t>"New collection == No" but lacks a Repository or a Community</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -167,13 +164,25 @@
     <t>Community</t>
   </si>
   <si>
-    <t>A collection with more than one Community or Repository</t>
-  </si>
-  <si>
     <t>Repository</t>
   </si>
   <si>
     <t>Invalid collection name '#N/A'</t>
+  </si>
+  <si>
+    <t>eProcurement</t>
+  </si>
+  <si>
+    <t>asset_release as solution in new collection</t>
+  </si>
+  <si>
+    <t>project_project as solution in new collection</t>
+  </si>
+  <si>
+    <t>More than one Community or Repository</t>
+  </si>
+  <si>
+    <t>No Repository or Community</t>
   </si>
 </sst>
 </file>
@@ -329,9 +338,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -435,7 +462,7 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="28">
+  <cellStyles count="46">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -449,6 +476,15 @@
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -462,6 +498,15 @@
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="1"/>
   </cellStyles>
@@ -822,8 +867,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A2:AA11" totalsRowShown="0" headerRowDxfId="24">
-  <autoFilter ref="A2:AA11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A2:AA13" totalsRowShown="0" headerRowDxfId="24">
+  <autoFilter ref="A2:AA13"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1126,7 +1171,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:AA11"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -1136,7 +1181,7 @@
   <cols>
     <col min="1" max="1" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="59.5" style="1" customWidth="1"/>
     <col min="5" max="6" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="1" bestFit="1" customWidth="1"/>
@@ -1279,10 +1324,10 @@
         <v>60735</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>3</v>
@@ -1291,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.15">
@@ -1302,10 +1347,10 @@
         <v>99999999</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="1" t="s">
@@ -1315,7 +1360,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
@@ -1340,13 +1385,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>39</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="1" t="s">
@@ -1356,7 +1401,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
@@ -1384,10 +1429,10 @@
         <v>157729</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="1" t="s">
@@ -1397,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
@@ -1425,7 +1470,7 @@
         <v>58729</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="e">
         <v>#N/A</v>
@@ -1438,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
@@ -1466,17 +1511,17 @@
         <v>60736</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
@@ -1498,16 +1543,16 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A9" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="20">
         <v>156207</v>
       </c>
       <c r="C9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="1" t="s">
@@ -1517,7 +1562,7 @@
         <v>#N/A</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
@@ -1539,16 +1584,16 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A10" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="20">
         <v>145807</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="1" t="s">
@@ -1558,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
@@ -1580,16 +1625,16 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A11" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="20">
         <v>105945</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="21" t="s">
@@ -1599,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
@@ -1619,6 +1664,88 @@
       <c r="Y11" s="27"/>
       <c r="AA11" s="19"/>
     </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A12" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="20">
+        <v>58694</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
+      <c r="AA12" s="19"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A13" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="20">
+        <v>26863</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="AA13" s="19"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
ISAICP-3181: Log wrong usage of Software (project) instead of Project (project_project).
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$13</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
   <si>
     <t>No</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>Invalid</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Software instead of Project</t>
   </si>
 </sst>
 </file>
@@ -254,7 +260,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -302,6 +308,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -338,7 +345,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="50">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -363,6 +370,7 @@
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -657,8 +665,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q12" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:Q12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q13" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:Q13"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -951,7 +959,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1389,17 +1397,53 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="7"/>
     </row>
+    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="4">
+        <v>87737</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="7"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M9" r:id="rId1"/>
     <hyperlink ref="M11" r:id="rId2"/>
     <hyperlink ref="M12" r:id="rId3"/>
     <hyperlink ref="M10" r:id="rId4"/>
+    <hyperlink ref="M13" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3230: Add 'document' casses to Excel testing file.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$20</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="54">
   <si>
     <t>No</t>
   </si>
@@ -159,6 +159,42 @@
   </si>
   <si>
     <t>Software instead of Project</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>Factsheet</t>
+  </si>
+  <si>
+    <t>Factsheet to Document (type=factsheet)</t>
+  </si>
+  <si>
+    <t>Legal document</t>
+  </si>
+  <si>
+    <t>Legal document to Document (type=legal)</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Presentation to Document (type=presentation)</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Case to Document (type=case)</t>
+  </si>
+  <si>
+    <t>Document with URL and file (file wins)</t>
+  </si>
+  <si>
+    <t>Document with URL</t>
+  </si>
+  <si>
+    <t>Document with file</t>
   </si>
 </sst>
 </file>
@@ -236,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -259,8 +295,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -311,8 +360,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -344,8 +416,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -371,6 +454,29 @@
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -665,8 +771,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q13" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:Q13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q20" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:Q20"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -959,7 +1065,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -969,7 +1075,7 @@
   <cols>
     <col min="1" max="1" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="31.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="1" bestFit="1" customWidth="1"/>
@@ -1432,6 +1538,251 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="7"/>
     </row>
+    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="13">
+        <v>139528</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="17">
+        <v>42233</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="7"/>
+    </row>
+    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="17">
+        <v>138766</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="17">
+        <v>133560</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="15">
+        <v>53012</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="16"/>
+    </row>
+    <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="4">
+        <v>63578</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="7"/>
+    </row>
+    <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="4">
+        <v>155691</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="7"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M9" r:id="rId1"/>
@@ -1439,11 +1790,18 @@
     <hyperlink ref="M12" r:id="rId3"/>
     <hyperlink ref="M10" r:id="rId4"/>
     <hyperlink ref="M13" r:id="rId5"/>
+    <hyperlink ref="M14" r:id="rId6"/>
+    <hyperlink ref="M18" r:id="rId7"/>
+    <hyperlink ref="M19" r:id="rId8"/>
+    <hyperlink ref="M20" r:id="rId9"/>
+    <hyperlink ref="M17" r:id="rId10"/>
+    <hyperlink ref="M15" r:id="rId11"/>
+    <hyperlink ref="M16" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3253: Switch cardinality for spatial coverage, in News, to unlimited. Add test coverage for 'news' migration.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$22</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="57">
   <si>
     <t>No</t>
   </si>
@@ -195,6 +195,15 @@
   </si>
   <si>
     <t>Document with file</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>News with 2 countries</t>
+  </si>
+  <si>
+    <t>News in Europe as country and Athens as city</t>
   </si>
 </sst>
 </file>
@@ -309,7 +318,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -357,6 +366,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -428,7 +440,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="76">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -477,6 +489,9 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -771,8 +786,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q20" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:Q20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q22" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:Q22"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1065,7 +1080,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1783,6 +1798,76 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="7"/>
     </row>
+    <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="4">
+        <v>27607</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="7"/>
+    </row>
+    <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="4">
+        <v>155894</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="7"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M9" r:id="rId1"/>
@@ -1797,11 +1882,13 @@
     <hyperlink ref="M17" r:id="rId10"/>
     <hyperlink ref="M15" r:id="rId11"/>
     <hyperlink ref="M16" r:id="rId12"/>
+    <hyperlink ref="M21" r:id="rId13"/>
+    <hyperlink ref="M22" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3220: Add newsletter migration test coverage.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$23</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="58">
   <si>
     <t>No</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>News in Europe as country and Athens as city</t>
+  </si>
+  <si>
+    <t>Newsletter</t>
   </si>
 </sst>
 </file>
@@ -318,7 +321,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="76">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -366,6 +369,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -440,7 +444,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="76">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -492,6 +496,7 @@
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -786,8 +791,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q22" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:Q22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q23" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:Q23"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1080,7 +1085,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1868,6 +1873,41 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="7"/>
     </row>
+    <row r="23" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="4">
+        <v>152066</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="7"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M9" r:id="rId1"/>
@@ -1884,11 +1924,12 @@
     <hyperlink ref="M16" r:id="rId12"/>
     <hyperlink ref="M21" r:id="rId13"/>
     <hyperlink ref="M22" r:id="rId14"/>
+    <hyperlink ref="M23" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
   <tableParts count="1">
-    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3265: The Issues migrated to the Discussion should be linked to the Solution and not to the Collection
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -321,7 +321,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -369,6 +369,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -444,7 +445,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="78">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -497,6 +498,7 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1493,7 +1495,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="4">
-        <v>26863</v>
+        <v>49860</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
ISAICP-3272: Test coverage for 'event' migration.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$24</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="60">
   <si>
     <t>No</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>Newsletter</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Event with image</t>
   </si>
 </sst>
 </file>
@@ -321,7 +327,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="78">
+  <cellStyleXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -369,6 +375,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -445,7 +453,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="78">
+  <cellStyles count="80">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -499,6 +507,8 @@
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -793,8 +803,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q23" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:Q23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q24" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:Q24"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1087,7 +1097,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1910,6 +1920,41 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="7"/>
     </row>
+    <row r="24" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="4">
+        <v>145278</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="7"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M9" r:id="rId1"/>
@@ -1927,11 +1972,12 @@
     <hyperlink ref="M21" r:id="rId13"/>
     <hyperlink ref="M22" r:id="rId14"/>
     <hyperlink ref="M23" r:id="rId15"/>
+    <hyperlink ref="M24" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
   <tableParts count="1">
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3272: Add 2 new collection test cases. Reorganise 'mapping' and 'prepare' assertions.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$26</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="68">
   <si>
     <t>No</t>
   </si>
@@ -213,13 +213,37 @@
   </si>
   <si>
     <t>Event with image</t>
+  </si>
+  <si>
+    <t>Repository as base for collection</t>
+  </si>
+  <si>
+    <t>Open government</t>
+  </si>
+  <si>
+    <t>baby.doe@example.com</t>
+  </si>
+  <si>
+    <t>Community as base for collection</t>
+  </si>
+  <si>
+    <t>Collection from Repository</t>
+  </si>
+  <si>
+    <t>Collection from Community</t>
+  </si>
+  <si>
+    <t>Collaboration</t>
+  </si>
+  <si>
+    <t>jbloggs@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +293,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -290,7 +320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -326,8 +356,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF5B9BD5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF5B9BD5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5B9BD5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="80">
+  <cellStyleXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -408,8 +453,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -452,8 +505,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="80">
+  <cellStyles count="88">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -509,6 +567,14 @@
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -803,8 +869,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q24" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:Q24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q26" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:Q26"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1097,7 +1163,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1116,7 +1182,7 @@
     <col min="10" max="10" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -1954,6 +2020,76 @@
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="7"/>
+    </row>
+    <row r="25" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="18">
+        <v>59642</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="7"/>
+    </row>
+    <row r="26" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="13">
+        <v>42436</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1973,11 +2109,13 @@
     <hyperlink ref="M22" r:id="rId14"/>
     <hyperlink ref="M23" r:id="rId15"/>
     <hyperlink ref="M24" r:id="rId16"/>
+    <hyperlink ref="M26" r:id="rId17"/>
+    <hyperlink ref="M25" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3272: Add test coverage for 'collection' migration.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="69">
   <si>
     <t>No</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>jbloggs@example.com</t>
+  </si>
+  <si>
+    <t>Abstract for a new collection</t>
   </si>
 </sst>
 </file>
@@ -372,7 +375,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="88">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -461,8 +464,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -510,8 +528,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="88">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -575,6 +596,21 @@
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -761,7 +797,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1215,7 +1251,7 @@
       <c r="H1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="21" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="9" t="s">
@@ -1289,7 +1325,6 @@
       <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -1322,7 +1357,6 @@
       <c r="H4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -1355,7 +1389,6 @@
       <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -1388,7 +1421,6 @@
       <c r="H6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -1418,7 +1450,6 @@
       <c r="H7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -1451,7 +1482,6 @@
       <c r="H8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -1484,7 +1514,6 @@
       <c r="H9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -1519,7 +1548,6 @@
       <c r="H10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1554,7 +1582,9 @@
       <c r="H11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -1589,7 +1619,9 @@
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="3"/>
+      <c r="I12" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1624,7 +1656,9 @@
       <c r="H13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1659,7 +1693,9 @@
       <c r="H14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="3"/>
+      <c r="I14" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1694,7 +1730,9 @@
       <c r="H15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="3"/>
+      <c r="I15" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1729,7 +1767,9 @@
       <c r="H16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="3"/>
+      <c r="I16" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1764,7 +1804,9 @@
       <c r="H17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="3"/>
+      <c r="I17" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1799,7 +1841,9 @@
       <c r="H18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="3"/>
+      <c r="I18" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1834,7 +1878,9 @@
       <c r="H19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="3"/>
+      <c r="I19" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1869,7 +1915,9 @@
       <c r="H20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="3"/>
+      <c r="I20" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1904,7 +1952,9 @@
       <c r="H21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1939,7 +1989,9 @@
       <c r="H22" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I22" s="3"/>
+      <c r="I22" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1974,7 +2026,9 @@
       <c r="H23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="3"/>
+      <c r="I23" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -2009,7 +2063,9 @@
       <c r="H24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I24" s="3"/>
+      <c r="I24" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -2044,7 +2100,6 @@
       <c r="H25" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -2061,7 +2116,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="13">
-        <v>42436</v>
+        <v>149141</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>63</v>
@@ -2079,7 +2134,6 @@
       <c r="H26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>

</xml_diff>

<commit_message>
New mapping file: Add new file versions.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -80,9 +80,6 @@
     <t>Type of content item</t>
   </si>
   <si>
-    <t>Content item status</t>
-  </si>
-  <si>
     <t>Migrate</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>Collection Owner</t>
   </si>
   <si>
-    <t>Collection status</t>
-  </si>
-  <si>
     <t>joeroe@example.com</t>
   </si>
   <si>
@@ -240,6 +234,12 @@
   </si>
   <si>
     <t>Abstract for a new collection</t>
+  </si>
+  <si>
+    <t>Collection state</t>
+  </si>
+  <si>
+    <t>Content item state</t>
   </si>
 </sst>
 </file>
@@ -926,8 +926,8 @@
     <tableColumn id="9" name="Collection Owner" dataDxfId="4" dataCellStyle="Normale 2"/>
     <tableColumn id="25" name="Elibrary Creation" dataDxfId="3"/>
     <tableColumn id="26" name="Pre Moderation" dataDxfId="2"/>
-    <tableColumn id="13" name="Collection status" dataDxfId="1"/>
-    <tableColumn id="28" name="Content item status" dataDxfId="0" dataCellStyle="Normale 2"/>
+    <tableColumn id="13" name="Collection state" dataDxfId="1"/>
+    <tableColumn id="28" name="Content item state" dataDxfId="0" dataCellStyle="Normale 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1201,8 +1201,8 @@
   </sheetPr>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1231,7 +1231,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>13</v>
@@ -1249,7 +1249,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="21" t="s">
         <v>8</v>
@@ -1264,7 +1264,7 @@
         <v>6</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N1" s="9" t="s">
         <v>5</v>
@@ -1273,10 +1273,10 @@
         <v>4</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>15</v>
+        <v>67</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
@@ -1287,10 +1287,10 @@
         <v>60735</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
@@ -1299,7 +1299,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
@@ -1310,20 +1310,20 @@
         <v>99999999</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1339,23 +1339,23 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1374,10 +1374,10 @@
         <v>157729</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="1" t="s">
@@ -1387,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1406,7 +1406,7 @@
         <v>58729</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="e">
         <v>#N/A</v>
@@ -1419,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1438,17 +1438,17 @@
         <v>60736</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1461,16 +1461,16 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4">
         <v>156207</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="1" t="s">
@@ -1480,7 +1480,7 @@
         <v>#N/A</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1493,16 +1493,16 @@
     </row>
     <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4">
         <v>145807</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="1" t="s">
@@ -1512,13 +1512,13 @@
         <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -1527,16 +1527,16 @@
     </row>
     <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4">
         <v>105945</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="5" t="s">
@@ -1546,13 +1546,13 @@
         <v>0</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
@@ -1567,29 +1567,29 @@
         <v>58694</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
@@ -1598,35 +1598,35 @@
     </row>
     <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4">
         <v>49860</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
@@ -1635,35 +1635,35 @@
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="4">
         <v>87737</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
@@ -1672,35 +1672,35 @@
     </row>
     <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="13">
         <v>139528</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
@@ -1709,35 +1709,35 @@
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="17">
         <v>42233</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
@@ -1746,35 +1746,35 @@
     </row>
     <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="17">
         <v>138766</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
@@ -1783,35 +1783,35 @@
     </row>
     <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" s="17">
         <v>133560</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -1820,35 +1820,35 @@
     </row>
     <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="15">
         <v>53012</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
@@ -1857,35 +1857,35 @@
     </row>
     <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4">
         <v>63578</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -1894,35 +1894,35 @@
     </row>
     <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="4">
         <v>155691</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -1931,35 +1931,35 @@
     </row>
     <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B21" s="4">
         <v>27607</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
@@ -1968,35 +1968,35 @@
     </row>
     <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B22" s="4">
         <v>155894</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
@@ -2005,35 +2005,35 @@
     </row>
     <row r="23" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" s="4">
         <v>152066</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -2042,35 +2042,35 @@
     </row>
     <row r="24" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" s="4">
         <v>145278</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -2079,32 +2079,32 @@
     </row>
     <row r="25" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="18">
         <v>59642</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
@@ -2113,32 +2113,32 @@
     </row>
     <row r="26" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="13">
         <v>149141</v>
       </c>
       <c r="C26" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>

</xml_diff>

<commit_message>
ISAICP-3068: State for 'collection' migration.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$28</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="73">
   <si>
     <t>No</t>
   </si>
@@ -240,6 +240,18 @@
   </si>
   <si>
     <t>Content item state</t>
+  </si>
+  <si>
+    <t>wrong</t>
+  </si>
+  <si>
+    <t>Archived collection</t>
+  </si>
+  <si>
+    <t>archived</t>
+  </si>
+  <si>
+    <t>Archived solution under archived collection</t>
   </si>
 </sst>
 </file>
@@ -375,7 +387,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -423,6 +435,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -532,7 +548,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -611,6 +627,10 @@
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -905,8 +925,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q26" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:Q26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q28" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:Q28"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1199,10 +1219,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1210,7 +1230,7 @@
     <col min="1" max="1" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" style="1" customWidth="1"/>
     <col min="5" max="6" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1363,7 +1383,9 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+      <c r="P4" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="Q4" s="7"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.15">
@@ -2144,6 +2166,76 @@
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="7"/>
+    </row>
+    <row r="27" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4">
+        <v>144326</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q27" s="7"/>
+    </row>
+    <row r="28" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4">
+        <v>76726</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2165,11 +2257,13 @@
     <hyperlink ref="M24" r:id="rId16"/>
     <hyperlink ref="M26" r:id="rId17"/>
     <hyperlink ref="M25" r:id="rId18"/>
+    <hyperlink ref="M27" r:id="rId19"/>
+    <hyperlink ref="M28" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3068: State for 'solution' migration.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="76">
   <si>
     <t>No</t>
   </si>
@@ -252,6 +252,15 @@
   </si>
   <si>
     <t>Archived solution under archived collection</t>
+  </si>
+  <si>
+    <t>proposed</t>
+  </si>
+  <si>
+    <t>needs_update</t>
+  </si>
+  <si>
+    <t>draft</t>
   </si>
 </sst>
 </file>
@@ -387,7 +396,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -435,6 +444,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -548,7 +561,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -631,6 +644,10 @@
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1616,7 +1633,9 @@
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="7"/>
+      <c r="Q11" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -1727,7 +1746,9 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="7"/>
+      <c r="Q14" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -1986,7 +2007,9 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="7"/>
+      <c r="Q21" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">

</xml_diff>

<commit_message>
ISAICP-3068: State for 'release' migration.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -1633,9 +1633,7 @@
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" t="s">
-        <v>73</v>
-      </c>
+      <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -1672,7 +1670,9 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-      <c r="Q12" s="7"/>
+      <c r="Q12" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">

</xml_diff>

<commit_message>
ISAICP-3068: Add 'contact' migration test coverage.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$29</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="77">
   <si>
     <t>No</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>draft</t>
+  </si>
+  <si>
+    <t>asset_release with contact point</t>
   </si>
 </sst>
 </file>
@@ -396,7 +399,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -444,6 +447,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -561,7 +565,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="112">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -648,6 +652,7 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -942,8 +947,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q28" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:Q28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q29" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:Q29"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1236,7 +1241,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2260,6 +2265,40 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="7"/>
     </row>
+    <row r="29" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4">
+        <v>102713</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="7"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M9" r:id="rId1"/>
@@ -2282,11 +2321,12 @@
     <hyperlink ref="M25" r:id="rId18"/>
     <hyperlink ref="M27" r:id="rId19"/>
     <hyperlink ref="M28" r:id="rId20"/>
+    <hyperlink ref="M29" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix nid case in mapping file and migration.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -134,9 +134,6 @@
     <t>No Repository or Community</t>
   </si>
   <si>
-    <t>nid</t>
-  </si>
-  <si>
     <t>Collection Owner</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>asset_release with contact point</t>
+  </si>
+  <si>
+    <t>Nid</t>
   </si>
 </sst>
 </file>
@@ -954,7 +954,7 @@
   </sortState>
   <tableColumns count="17">
     <tableColumn id="20" name="Type of content item" dataDxfId="15"/>
-    <tableColumn id="18" name="nid" dataDxfId="14"/>
+    <tableColumn id="18" name="Nid" dataDxfId="14"/>
     <tableColumn id="1" name="Title of content item" dataDxfId="13"/>
     <tableColumn id="10" name="Collection_Name"/>
     <tableColumn id="3" name="Policy domain 1" dataDxfId="12"/>
@@ -1243,9 +1243,7 @@
   </sheetPr>
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1273,7 +1271,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>13</v>
@@ -1306,7 +1304,7 @@
         <v>6</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N1" s="9" t="s">
         <v>5</v>
@@ -1315,10 +1313,10 @@
         <v>4</v>
       </c>
       <c r="P1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
@@ -1362,7 +1360,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>16</v>
@@ -1406,7 +1404,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q4" s="7"/>
     </row>
@@ -1562,7 +1560,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -1596,7 +1594,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
@@ -1627,13 +1625,13 @@
         <v>16</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
@@ -1664,30 +1662,30 @@
         <v>16</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4">
         <v>87737</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
@@ -1703,13 +1701,13 @@
         <v>16</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
@@ -1718,13 +1716,13 @@
     </row>
     <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="13">
         <v>139528</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
@@ -1740,30 +1738,30 @@
         <v>16</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="17">
         <v>42233</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
@@ -1779,13 +1777,13 @@
         <v>16</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
@@ -1794,13 +1792,13 @@
     </row>
     <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="17">
         <v>138766</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -1816,13 +1814,13 @@
         <v>16</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
@@ -1831,13 +1829,13 @@
     </row>
     <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="17">
         <v>133560</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
@@ -1853,13 +1851,13 @@
         <v>16</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -1868,13 +1866,13 @@
     </row>
     <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="15">
         <v>53012</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
@@ -1890,13 +1888,13 @@
         <v>16</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
@@ -1905,13 +1903,13 @@
     </row>
     <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="4">
         <v>63578</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
@@ -1927,13 +1925,13 @@
         <v>16</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -1942,13 +1940,13 @@
     </row>
     <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="4">
         <v>155691</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
@@ -1964,13 +1962,13 @@
         <v>16</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -1979,13 +1977,13 @@
     </row>
     <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="4">
         <v>27607</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
@@ -2001,30 +1999,30 @@
         <v>16</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="4">
         <v>155894</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>9</v>
@@ -2040,13 +2038,13 @@
         <v>16</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
@@ -2055,13 +2053,13 @@
     </row>
     <row r="23" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="4">
         <v>152066</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
@@ -2077,13 +2075,13 @@
         <v>16</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -2092,13 +2090,13 @@
     </row>
     <row r="24" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="4">
         <v>145278</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>9</v>
@@ -2114,13 +2112,13 @@
         <v>16</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -2135,14 +2133,14 @@
         <v>59642</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>0</v>
@@ -2154,7 +2152,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
@@ -2169,14 +2167,14 @@
         <v>149141</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>0</v>
@@ -2188,7 +2186,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
@@ -2203,14 +2201,14 @@
         <v>144326</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>0</v>
@@ -2222,12 +2220,12 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q27" s="7"/>
     </row>
@@ -2239,14 +2237,14 @@
         <v>76726</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>0</v>
@@ -2258,7 +2256,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
@@ -2273,14 +2271,14 @@
         <v>102713</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>0</v>
@@ -2292,7 +2290,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>

</xml_diff>

<commit_message>
ISAICP-3188: Migrate documents with unlimited cardinality file field.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$31</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="79">
   <si>
     <t>No</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>Nid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Document with URL and multiple files</t>
   </si>
 </sst>
 </file>
@@ -399,7 +405,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="112">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -447,6 +453,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -565,7 +574,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="112">
+  <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -653,6 +662,9 @@
     <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -947,8 +959,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q29" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:Q29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q31" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:Q31"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1241,9 +1253,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2297,6 +2311,59 @@
       <c r="P29" s="3"/>
       <c r="Q29" s="7"/>
     </row>
+    <row r="30" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="4">
+        <v>125548</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="7"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="6"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="7"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M9" r:id="rId1"/>
@@ -2320,11 +2387,12 @@
     <hyperlink ref="M27" r:id="rId19"/>
     <hyperlink ref="M28" r:id="rId20"/>
     <hyperlink ref="M29" r:id="rId21"/>
+    <hyperlink ref="M30" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
   <tableParts count="1">
-    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId24"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3199: Migrate News, Event & Discussion field Documentation/Attachments.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$33</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="81">
   <si>
     <t>No</t>
   </si>
@@ -266,10 +266,16 @@
     <t>Nid</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Document with URL and multiple files</t>
+  </si>
+  <si>
+    <t>Project having Issue with &gt; 1 files</t>
+  </si>
+  <si>
+    <t>Event with &gt; 1 files</t>
+  </si>
+  <si>
+    <t>News with &gt; 1 files</t>
   </si>
 </sst>
 </file>
@@ -405,7 +411,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -453,6 +459,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -574,7 +584,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -665,6 +675,10 @@
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -959,8 +973,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q31" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:Q31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q33" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:Q33"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1253,7 +1267,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2319,7 +2333,7 @@
         <v>125548</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>69</v>
@@ -2345,24 +2359,107 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="7"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
+    <row r="31" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="4">
+        <v>42444</v>
+      </c>
       <c r="C31" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="6"/>
+      <c r="F31" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="12"/>
+      <c r="M31" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
       <c r="Q31" s="7"/>
+    </row>
+    <row r="32" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="4">
+        <v>150255</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="7"/>
+    </row>
+    <row r="33" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="4">
+        <v>65803</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2388,11 +2485,14 @@
     <hyperlink ref="M28" r:id="rId20"/>
     <hyperlink ref="M29" r:id="rId21"/>
     <hyperlink ref="M30" r:id="rId22"/>
+    <hyperlink ref="M31" r:id="rId23"/>
+    <hyperlink ref="M32" r:id="rId24"/>
+    <hyperlink ref="M33" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
   <tableParts count="1">
-    <tablePart r:id="rId24"/>
+    <tablePart r:id="rId27"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3060: Add the new content mapping file (v1.12).
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$Q$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$33</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="87">
   <si>
     <t>No</t>
   </si>
@@ -276,13 +276,31 @@
   </si>
   <si>
     <t>News with &gt; 1 files</t>
+  </si>
+  <si>
+    <t>Owner name</t>
+  </si>
+  <si>
+    <t>Owner type</t>
+  </si>
+  <si>
+    <t>Text owner 1</t>
+  </si>
+  <si>
+    <t>SupraNationalAuthority</t>
+  </si>
+  <si>
+    <t>Text owner 2</t>
+  </si>
+  <si>
+    <t>Academia-ScientificOrganisation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,8 +356,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,8 +383,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -410,6 +441,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF5B9BD5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5B9BD5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -532,7 +576,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -582,6 +626,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="119">
@@ -705,7 +758,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="19">
     <dxf>
       <font>
         <b val="0"/>
@@ -722,6 +775,42 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -973,24 +1062,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:Q33" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:Q33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S33" totalsRowShown="0" headerRowDxfId="18">
+  <autoFilter ref="A1:S33"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
-  <tableColumns count="17">
-    <tableColumn id="20" name="Type of content item" dataDxfId="15"/>
-    <tableColumn id="18" name="Nid" dataDxfId="14"/>
-    <tableColumn id="1" name="Title of content item" dataDxfId="13"/>
+  <tableColumns count="19">
+    <tableColumn id="20" name="Type of content item" dataDxfId="17"/>
+    <tableColumn id="18" name="Nid" dataDxfId="16"/>
+    <tableColumn id="1" name="Title of content item" dataDxfId="15"/>
     <tableColumn id="10" name="Collection_Name"/>
-    <tableColumn id="3" name="Policy domain 1" dataDxfId="12"/>
-    <tableColumn id="27" name="Policy domain 2" dataDxfId="11" dataCellStyle="Normale 2"/>
-    <tableColumn id="22" name="New collection" dataDxfId="10"/>
-    <tableColumn id="30" name="Migrate" dataDxfId="9" dataCellStyle="Normale 2"/>
-    <tableColumn id="12" name="Abstract" dataDxfId="8"/>
-    <tableColumn id="8" name="Logo" dataDxfId="7"/>
-    <tableColumn id="2" name="Banner" dataDxfId="6"/>
-    <tableColumn id="15" name="Owner" dataDxfId="5"/>
+    <tableColumn id="3" name="Policy domain 1" dataDxfId="14"/>
+    <tableColumn id="27" name="Policy domain 2" dataDxfId="13" dataCellStyle="Normale 2"/>
+    <tableColumn id="22" name="New collection" dataDxfId="12"/>
+    <tableColumn id="30" name="Migrate" dataDxfId="11" dataCellStyle="Normale 2"/>
+    <tableColumn id="12" name="Abstract" dataDxfId="10"/>
+    <tableColumn id="8" name="Logo" dataDxfId="9"/>
+    <tableColumn id="2" name="Banner" dataDxfId="8"/>
+    <tableColumn id="15" name="Owner" dataDxfId="7"/>
+    <tableColumn id="5" name="Owner name" dataDxfId="6" dataCellStyle="Normale 2"/>
+    <tableColumn id="4" name="Owner type" dataDxfId="5" dataCellStyle="Normale 2"/>
     <tableColumn id="9" name="Collection Owner" dataDxfId="4" dataCellStyle="Normale 2"/>
     <tableColumn id="25" name="Elibrary Creation" dataDxfId="3"/>
     <tableColumn id="26" name="Pre Moderation" dataDxfId="2"/>
@@ -1267,7 +1358,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1286,15 +1377,17 @@
     <col min="10" max="10" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.1640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" style="1" customWidth="1"/>
     <col min="16" max="16" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="24.1640625" style="1"/>
+    <col min="17" max="17" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="24.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1331,23 +1424,29 @@
       <c r="L1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1370,7 +1469,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1396,13 +1495,15 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="12"/>
+      <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="O3" s="12"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="7"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="7"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1431,12 +1532,14 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" s="7"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S4" s="7"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1466,9 +1569,11 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="7"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="7"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1498,9 +1603,11 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="7"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="7"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1527,9 +1634,11 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="7"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="7"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1555,13 +1664,15 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="7"/>
-    </row>
-    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="7"/>
+    </row>
+    <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1587,15 +1698,17 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="7"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -1621,15 +1734,17 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="7"/>
-    </row>
-    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="7"/>
+    </row>
+    <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -1658,15 +1773,17 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="7"/>
-    </row>
-    <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="7"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1695,17 +1812,23 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="11" t="s">
+      <c r="M12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="N12" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="O12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-      <c r="Q12" t="s">
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1734,15 +1857,17 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="7"/>
-    </row>
-    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="7"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -1771,17 +1896,19 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="11" t="s">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" t="s">
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -1810,15 +1937,17 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="11" t="s">
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="7"/>
-    </row>
-    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="7"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>39</v>
       </c>
@@ -1847,15 +1976,17 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="11" t="s">
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
       <c r="P16" s="3"/>
-      <c r="Q16" s="7"/>
-    </row>
-    <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="7"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -1884,15 +2015,17 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="11" t="s">
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
       <c r="P17" s="3"/>
-      <c r="Q17" s="7"/>
-    </row>
-    <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="7"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>40</v>
       </c>
@@ -1921,15 +2054,17 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="11" t="s">
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
       <c r="P18" s="14"/>
-      <c r="Q18" s="16"/>
-    </row>
-    <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="16"/>
+    </row>
+    <row r="19" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
@@ -1958,15 +2093,17 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="11" t="s">
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="7"/>
-    </row>
-    <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="7"/>
+    </row>
+    <row r="20" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
@@ -1995,15 +2132,17 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="7"/>
-    </row>
-    <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="7"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
@@ -2032,17 +2171,19 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="11" t="s">
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
       <c r="P21" s="3"/>
-      <c r="Q21" t="s">
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
@@ -2071,15 +2212,17 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="11" t="s">
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
       <c r="P22" s="3"/>
-      <c r="Q22" s="7"/>
-    </row>
-    <row r="23" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="7"/>
+    </row>
+    <row r="23" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>54</v>
       </c>
@@ -2108,15 +2251,17 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="11" t="s">
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
       <c r="P23" s="3"/>
-      <c r="Q23" s="7"/>
-    </row>
-    <row r="24" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="7"/>
+    </row>
+    <row r="24" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>55</v>
       </c>
@@ -2145,15 +2290,17 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="11" t="s">
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
       <c r="P24" s="3"/>
-      <c r="Q24" s="7"/>
-    </row>
-    <row r="25" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="7"/>
+    </row>
+    <row r="25" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
@@ -2179,15 +2326,17 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="20" t="s">
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
       <c r="P25" s="3"/>
-      <c r="Q25" s="7"/>
-    </row>
-    <row r="26" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="7"/>
+    </row>
+    <row r="26" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -2213,15 +2362,17 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="20" t="s">
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="7"/>
-    </row>
-    <row r="27" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="7"/>
+    </row>
+    <row r="27" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
@@ -2247,17 +2398,19 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="11" t="s">
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3" t="s">
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="Q27" s="7"/>
-    </row>
-    <row r="28" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="S27" s="7"/>
+    </row>
+    <row r="28" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>1</v>
       </c>
@@ -2283,15 +2436,17 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="11" t="s">
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
       <c r="P28" s="3"/>
-      <c r="Q28" s="7"/>
-    </row>
-    <row r="29" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="7"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>1</v>
       </c>
@@ -2317,15 +2472,17 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="11" t="s">
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="7"/>
-    </row>
-    <row r="30" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="7"/>
+    </row>
+    <row r="30" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -2351,15 +2508,17 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="11" t="s">
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
       <c r="P30" s="3"/>
-      <c r="Q30" s="7"/>
-    </row>
-    <row r="31" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="7"/>
+    </row>
+    <row r="31" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>23</v>
       </c>
@@ -2385,15 +2544,21 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="11" t="s">
+      <c r="M31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="N31" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="O31" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
       <c r="P31" s="3"/>
-      <c r="Q31" s="7"/>
-    </row>
-    <row r="32" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="7"/>
+    </row>
+    <row r="32" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>55</v>
       </c>
@@ -2419,15 +2584,17 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
-      <c r="M32" s="11" t="s">
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
       <c r="P32" s="3"/>
-      <c r="Q32" s="7"/>
-    </row>
-    <row r="33" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="7"/>
+    </row>
+    <row r="33" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>51</v>
       </c>
@@ -2453,41 +2620,43 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="11" t="s">
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
       <c r="P33" s="3"/>
-      <c r="Q33" s="7"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M9" r:id="rId1"/>
-    <hyperlink ref="M11" r:id="rId2"/>
-    <hyperlink ref="M12" r:id="rId3"/>
-    <hyperlink ref="M10" r:id="rId4"/>
-    <hyperlink ref="M13" r:id="rId5"/>
-    <hyperlink ref="M14" r:id="rId6"/>
-    <hyperlink ref="M18" r:id="rId7"/>
-    <hyperlink ref="M19" r:id="rId8"/>
-    <hyperlink ref="M20" r:id="rId9"/>
-    <hyperlink ref="M17" r:id="rId10"/>
-    <hyperlink ref="M15" r:id="rId11"/>
-    <hyperlink ref="M16" r:id="rId12"/>
-    <hyperlink ref="M21" r:id="rId13"/>
-    <hyperlink ref="M22" r:id="rId14"/>
-    <hyperlink ref="M23" r:id="rId15"/>
-    <hyperlink ref="M24" r:id="rId16"/>
-    <hyperlink ref="M26" r:id="rId17"/>
-    <hyperlink ref="M25" r:id="rId18"/>
-    <hyperlink ref="M27" r:id="rId19"/>
-    <hyperlink ref="M28" r:id="rId20"/>
-    <hyperlink ref="M29" r:id="rId21"/>
-    <hyperlink ref="M30" r:id="rId22"/>
-    <hyperlink ref="M31" r:id="rId23"/>
-    <hyperlink ref="M32" r:id="rId24"/>
-    <hyperlink ref="M33" r:id="rId25"/>
+    <hyperlink ref="O9" r:id="rId1"/>
+    <hyperlink ref="O11" r:id="rId2"/>
+    <hyperlink ref="O12" r:id="rId3"/>
+    <hyperlink ref="O10" r:id="rId4"/>
+    <hyperlink ref="O13" r:id="rId5"/>
+    <hyperlink ref="O14" r:id="rId6"/>
+    <hyperlink ref="O18" r:id="rId7"/>
+    <hyperlink ref="O19" r:id="rId8"/>
+    <hyperlink ref="O20" r:id="rId9"/>
+    <hyperlink ref="O17" r:id="rId10"/>
+    <hyperlink ref="O15" r:id="rId11"/>
+    <hyperlink ref="O16" r:id="rId12"/>
+    <hyperlink ref="O21" r:id="rId13"/>
+    <hyperlink ref="O22" r:id="rId14"/>
+    <hyperlink ref="O23" r:id="rId15"/>
+    <hyperlink ref="O24" r:id="rId16"/>
+    <hyperlink ref="O26" r:id="rId17"/>
+    <hyperlink ref="O25" r:id="rId18"/>
+    <hyperlink ref="O27" r:id="rId19"/>
+    <hyperlink ref="O28" r:id="rId20"/>
+    <hyperlink ref="O29" r:id="rId21"/>
+    <hyperlink ref="O30" r:id="rId22"/>
+    <hyperlink ref="O31" r:id="rId23"/>
+    <hyperlink ref="O32" r:id="rId24"/>
+    <hyperlink ref="O33" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>

</xml_diff>

<commit_message>
ISAICP-3060: Add the new 'owner_text' migration.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -284,16 +284,16 @@
     <t>Owner type</t>
   </si>
   <si>
-    <t>Text owner 1</t>
-  </si>
-  <si>
     <t>SupraNationalAuthority</t>
   </si>
   <si>
-    <t>Text owner 2</t>
-  </si>
-  <si>
     <t>Academia-ScientificOrganisation</t>
+  </si>
+  <si>
+    <t>Dark Side of The Force</t>
+  </si>
+  <si>
+    <t>ACME University</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -503,6 +503,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -637,7 +642,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="124">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -732,6 +737,11 @@
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1377,7 +1387,7 @@
     <col min="10" max="10" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" style="1" customWidth="1"/>
     <col min="15" max="15" width="21.1640625" style="1" customWidth="1"/>
     <col min="16" max="16" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -1812,11 +1822,11 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="3" t="s">
+      <c r="M12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" s="24" t="s">
         <v>83</v>
-      </c>
-      <c r="N12" s="24" t="s">
-        <v>84</v>
       </c>
       <c r="O12" s="11" t="s">
         <v>35</v>
@@ -2545,10 +2555,10 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N31" s="24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O31" s="11" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
ISAICP-3060: Detect type mismatch in Excel file.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$34</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="87">
   <si>
     <t>No</t>
   </si>
@@ -146,9 +146,6 @@
     <t>Invalid</t>
   </si>
   <si>
-    <t>Software</t>
-  </si>
-  <si>
     <t>Software instead of Project</t>
   </si>
   <si>
@@ -294,13 +291,16 @@
   </si>
   <si>
     <t>ACME University</t>
+  </si>
+  <si>
+    <t>News declared as newsletter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +362,11 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
     </font>
   </fonts>
   <fills count="5">
@@ -455,7 +460,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="124">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -580,8 +585,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -641,8 +647,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="124">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -742,6 +749,7 @@
     <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1072,8 +1080,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S33" totalsRowShown="0" headerRowDxfId="18">
-  <autoFilter ref="A1:S33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S34" totalsRowShown="0" headerRowDxfId="18">
+  <autoFilter ref="A1:S34"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1368,7 +1376,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1402,7 +1410,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>13</v>
@@ -1435,10 +1443,10 @@
         <v>6</v>
       </c>
       <c r="M1" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="23" t="s">
         <v>81</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>82</v>
       </c>
       <c r="O1" s="8" t="s">
         <v>33</v>
@@ -1450,10 +1458,10 @@
         <v>4</v>
       </c>
       <c r="R1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
@@ -1545,7 +1553,7 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S4" s="7"/>
     </row>
@@ -1778,7 +1786,7 @@
         <v>16</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1817,16 +1825,16 @@
         <v>16</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O12" s="11" t="s">
         <v>35</v>
@@ -1835,18 +1843,18 @@
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4">
         <v>87737</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
@@ -1862,7 +1870,7 @@
         <v>16</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1879,13 +1887,13 @@
     </row>
     <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="13">
         <v>139528</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
@@ -1901,7 +1909,7 @@
         <v>16</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1915,18 +1923,18 @@
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="17">
         <v>42233</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
@@ -1942,7 +1950,7 @@
         <v>16</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1959,13 +1967,13 @@
     </row>
     <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="17">
         <v>138766</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -1981,7 +1989,7 @@
         <v>16</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1998,13 +2006,13 @@
     </row>
     <row r="17" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="17">
         <v>133560</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
@@ -2020,7 +2028,7 @@
         <v>16</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -2037,13 +2045,13 @@
     </row>
     <row r="18" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="15">
         <v>53012</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
@@ -2059,7 +2067,7 @@
         <v>16</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -2076,13 +2084,13 @@
     </row>
     <row r="19" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="4">
         <v>63578</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
@@ -2098,7 +2106,7 @@
         <v>16</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -2115,13 +2123,13 @@
     </row>
     <row r="20" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="4">
         <v>155691</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
@@ -2137,7 +2145,7 @@
         <v>16</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -2154,13 +2162,13 @@
     </row>
     <row r="21" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="4">
         <v>27607</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
@@ -2176,7 +2184,7 @@
         <v>16</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -2190,18 +2198,18 @@
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4">
         <v>155894</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>9</v>
@@ -2217,7 +2225,7 @@
         <v>16</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -2234,13 +2242,13 @@
     </row>
     <row r="23" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="4">
         <v>152066</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
@@ -2256,7 +2264,7 @@
         <v>16</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -2273,13 +2281,13 @@
     </row>
     <row r="24" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="4">
         <v>145278</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>9</v>
@@ -2295,7 +2303,7 @@
         <v>16</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2318,14 +2326,14 @@
         <v>59642</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>0</v>
@@ -2339,7 +2347,7 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -2354,14 +2362,14 @@
         <v>149141</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>0</v>
@@ -2375,7 +2383,7 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -2384,20 +2392,20 @@
     </row>
     <row r="27" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B27" s="4">
         <v>144326</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>0</v>
@@ -2416,7 +2424,7 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S27" s="7"/>
     </row>
@@ -2428,14 +2436,14 @@
         <v>76726</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>0</v>
@@ -2464,14 +2472,14 @@
         <v>102713</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>0</v>
@@ -2494,20 +2502,20 @@
     </row>
     <row r="30" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4">
         <v>125548</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>0</v>
@@ -2536,14 +2544,14 @@
         <v>42444</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>0</v>
@@ -2555,10 +2563,10 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N31" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O31" s="11" t="s">
         <v>35</v>
@@ -2570,20 +2578,20 @@
     </row>
     <row r="32" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="4">
         <v>150255</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>0</v>
@@ -2606,20 +2614,20 @@
     </row>
     <row r="33" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B33" s="4">
         <v>65803</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>0</v>
@@ -2639,6 +2647,40 @@
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="7"/>
+    </row>
+    <row r="34" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="25">
+        <v>156973</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
ISAICP-3060: Migrate text owner references in solutions and colelctions.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="88">
   <si>
     <t>No</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>News declared as newsletter</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -508,6 +511,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -649,7 +654,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="127">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -750,6 +755,8 @@
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1829,7 +1836,9 @@
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="L12" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="M12" s="1" t="s">
         <v>84</v>
       </c>
@@ -2489,7 +2498,9 @@
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
+      <c r="L29" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="11" t="s">

</xml_diff>

<commit_message>
ISAICP-3218: Migrate 'reply' comments together with attachments.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$35</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="89">
   <si>
     <t>No</t>
   </si>
@@ -297,13 +297,16 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>project with discussions having replies with files</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,11 +369,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -398,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -419,19 +417,6 @@
       <bottom style="thin">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right style="thin">
-        <color theme="4"/>
-      </right>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -463,7 +448,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -591,70 +576,79 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -757,6 +751,8 @@
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -783,204 +779,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <font>
         <b val="0"/>
@@ -998,56 +797,10 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="top" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1073,6 +826,256 @@
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="top" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1087,31 +1090,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S34" totalsRowShown="0" headerRowDxfId="18">
-  <autoFilter ref="A1:S34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S35" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:S35"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="20" name="Type of content item" dataDxfId="17"/>
-    <tableColumn id="18" name="Nid" dataDxfId="16"/>
-    <tableColumn id="1" name="Title of content item" dataDxfId="15"/>
-    <tableColumn id="10" name="Collection_Name"/>
-    <tableColumn id="3" name="Policy domain 1" dataDxfId="14"/>
-    <tableColumn id="27" name="Policy domain 2" dataDxfId="13" dataCellStyle="Normale 2"/>
-    <tableColumn id="22" name="New collection" dataDxfId="12"/>
-    <tableColumn id="30" name="Migrate" dataDxfId="11" dataCellStyle="Normale 2"/>
-    <tableColumn id="12" name="Abstract" dataDxfId="10"/>
-    <tableColumn id="8" name="Logo" dataDxfId="9"/>
-    <tableColumn id="2" name="Banner" dataDxfId="8"/>
-    <tableColumn id="15" name="Owner" dataDxfId="7"/>
-    <tableColumn id="5" name="Owner name" dataDxfId="6" dataCellStyle="Normale 2"/>
-    <tableColumn id="4" name="Owner type" dataDxfId="5" dataCellStyle="Normale 2"/>
-    <tableColumn id="9" name="Collection Owner" dataDxfId="4" dataCellStyle="Normale 2"/>
-    <tableColumn id="25" name="Elibrary Creation" dataDxfId="3"/>
-    <tableColumn id="26" name="Pre Moderation" dataDxfId="2"/>
-    <tableColumn id="13" name="Collection state" dataDxfId="1"/>
-    <tableColumn id="28" name="Content item state" dataDxfId="0" dataCellStyle="Normale 2"/>
+    <tableColumn id="20" name="Type of content item" dataDxfId="20"/>
+    <tableColumn id="18" name="Nid" dataDxfId="0" dataCellStyle="Normale 2"/>
+    <tableColumn id="1" name="Title of content item" dataDxfId="19"/>
+    <tableColumn id="10" name="Collection_Name" dataDxfId="18"/>
+    <tableColumn id="3" name="Policy domain 1" dataDxfId="17"/>
+    <tableColumn id="27" name="Policy domain 2" dataDxfId="16" dataCellStyle="Normale 2"/>
+    <tableColumn id="22" name="New collection" dataDxfId="15"/>
+    <tableColumn id="30" name="Migrate" dataDxfId="14" dataCellStyle="Normale 2"/>
+    <tableColumn id="12" name="Abstract" dataDxfId="13"/>
+    <tableColumn id="8" name="Logo" dataDxfId="12"/>
+    <tableColumn id="2" name="Banner" dataDxfId="11"/>
+    <tableColumn id="15" name="Owner" dataDxfId="10"/>
+    <tableColumn id="5" name="Owner name" dataDxfId="9" dataCellStyle="Normale 2"/>
+    <tableColumn id="4" name="Owner type" dataDxfId="8" dataCellStyle="Normale 2"/>
+    <tableColumn id="9" name="Collection Owner" dataDxfId="7" dataCellStyle="Normale 2"/>
+    <tableColumn id="25" name="Elibrary Creation" dataDxfId="6"/>
+    <tableColumn id="26" name="Pre Moderation" dataDxfId="5"/>
+    <tableColumn id="13" name="Collection state" dataDxfId="4"/>
+    <tableColumn id="28" name="Content item state" dataDxfId="3" dataCellStyle="Normale 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1383,1315 +1386,1353 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="24.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="24.1640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38" style="1" customWidth="1"/>
-    <col min="5" max="6" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="21.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="24.1640625" style="1"/>
+    <col min="1" max="1" width="19.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="38" style="8" customWidth="1"/>
+    <col min="5" max="6" width="16.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" style="8" customWidth="1"/>
+    <col min="14" max="14" width="18.5" style="8" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" style="8" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="24.1640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:19" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="9">
         <v>60735</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+      <c r="H2" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="9">
         <v>99999999</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="7"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
+      <c r="H3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="12"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3" t="s">
+      <c r="G4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="S4" s="7"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
+      <c r="S4" s="12"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="9">
         <v>157729</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="7"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
+      <c r="H5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="12"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="9">
         <v>58729</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="e">
+      <c r="D6" s="8" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="7"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
+      <c r="H6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="12"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="9">
         <v>60736</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="7"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
+      <c r="G7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="12"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="9">
         <v>156207</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="3" t="e">
+      <c r="G8" s="10" t="e">
         <v>#N/A</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="7"/>
+      <c r="H8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="12"/>
     </row>
     <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="9">
         <v>145807</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="11" t="s">
+      <c r="H9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="7"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="12"/>
     </row>
     <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="9">
         <v>105945</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="10"/>
+      <c r="F10" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="11" t="s">
+      <c r="H10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="7"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="12"/>
     </row>
     <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="9">
         <v>58694</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="5" t="s">
+      <c r="E11" s="10"/>
+      <c r="F11" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="G11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="11" t="s">
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="7"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="12"/>
     </row>
     <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="9">
         <v>49860</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="5" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="H12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3" t="s">
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="O12" s="11" t="s">
+      <c r="O12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" t="s">
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="17" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="9">
         <v>87737</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="5" t="s">
+      <c r="E13" s="10"/>
+      <c r="F13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="G13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="11" t="s">
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="7"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="12"/>
     </row>
     <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="9">
         <v>139528</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="5" t="s">
+      <c r="E14" s="10"/>
+      <c r="F14" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="G14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="11" t="s">
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" t="s">
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="9">
         <v>42233</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="5" t="s">
+      <c r="E15" s="10"/>
+      <c r="F15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="G15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="11" t="s">
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="7"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="12"/>
     </row>
     <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="9">
         <v>138766</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="5" t="s">
+      <c r="E16" s="10"/>
+      <c r="F16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="G16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="11" t="s">
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="7"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="12"/>
     </row>
     <row r="17" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="9">
         <v>133560</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="5" t="s">
+      <c r="E17" s="10"/>
+      <c r="F17" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="1" t="s">
+      <c r="G17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="11" t="s">
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="7"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="12"/>
     </row>
     <row r="18" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="9">
         <v>53012</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="5" t="s">
+      <c r="E18" s="10"/>
+      <c r="F18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="G18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="11" t="s">
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="16"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="19"/>
     </row>
     <row r="19" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="9">
         <v>63578</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="10"/>
+      <c r="F19" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="G19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="11" t="s">
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="7"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="12"/>
     </row>
     <row r="20" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="9">
         <v>155691</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="5" t="s">
+      <c r="E20" s="10"/>
+      <c r="F20" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="1" t="s">
+      <c r="G20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="11" t="s">
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="7"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="12"/>
     </row>
     <row r="21" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="9">
         <v>27607</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="5" t="s">
+      <c r="E21" s="10"/>
+      <c r="F21" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="1" t="s">
+      <c r="G21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="11" t="s">
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" t="s">
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="17" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="9">
         <v>155894</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="5" t="s">
+      <c r="E22" s="10"/>
+      <c r="F22" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="1" t="s">
+      <c r="G22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="11" t="s">
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="7"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="12"/>
     </row>
     <row r="23" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="9">
         <v>152066</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="5" t="s">
+      <c r="E23" s="10"/>
+      <c r="F23" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="1" t="s">
+      <c r="G23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="11" t="s">
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="7"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="12"/>
     </row>
     <row r="24" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="9">
         <v>145278</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="5" t="s">
+      <c r="E24" s="10"/>
+      <c r="F24" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="1" t="s">
+      <c r="G24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="11" t="s">
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="7"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="12"/>
     </row>
     <row r="25" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="9">
         <v>59642</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="18" t="s">
+      <c r="E25" s="10"/>
+      <c r="F25" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="20" t="s">
+      <c r="H25" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="7"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="12"/>
     </row>
     <row r="26" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="9">
         <v>149141</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="18" t="s">
+      <c r="E26" s="10"/>
+      <c r="F26" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="20" t="s">
+      <c r="H26" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="7"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="12"/>
     </row>
     <row r="27" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="9">
         <v>144326</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="18" t="s">
+      <c r="E27" s="10"/>
+      <c r="F27" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="11" t="s">
+      <c r="H27" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3" t="s">
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="S27" s="7"/>
+      <c r="S27" s="12"/>
     </row>
     <row r="28" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="9">
         <v>76726</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="18" t="s">
+      <c r="E28" s="10"/>
+      <c r="F28" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="11" t="s">
+      <c r="H28" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="7"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="12"/>
     </row>
     <row r="29" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="9">
         <v>102713</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="18" t="s">
+      <c r="E29" s="10"/>
+      <c r="F29" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3" t="s">
+      <c r="H29" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="11" t="s">
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="7"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="12"/>
     </row>
     <row r="30" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="9">
         <v>125548</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="18" t="s">
+      <c r="E30" s="10"/>
+      <c r="F30" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="11" t="s">
+      <c r="H30" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="7"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="12"/>
     </row>
     <row r="31" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="9">
         <v>42444</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="18" t="s">
+      <c r="E31" s="10"/>
+      <c r="F31" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3" t="s">
+      <c r="H31" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="N31" s="24" t="s">
+      <c r="N31" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="O31" s="11" t="s">
+      <c r="O31" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="7"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="12"/>
     </row>
     <row r="32" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="9">
         <v>150255</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="18" t="s">
+      <c r="E32" s="10"/>
+      <c r="F32" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="11" t="s">
+      <c r="H32" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="7"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="12"/>
     </row>
     <row r="33" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="9">
         <v>65803</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="18" t="s">
+      <c r="E33" s="10"/>
+      <c r="F33" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H33" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="11" t="s">
+      <c r="H33" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="7"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="12"/>
     </row>
     <row r="34" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B34" s="9">
         <v>156973</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="18" t="s">
+      <c r="E34" s="10"/>
+      <c r="F34" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
-      <c r="S34" s="7"/>
+      <c r="H34" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="12"/>
+    </row>
+    <row r="35" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="9">
+        <v>63567</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2720,11 +2761,13 @@
     <hyperlink ref="O31" r:id="rId23"/>
     <hyperlink ref="O32" r:id="rId24"/>
     <hyperlink ref="O33" r:id="rId25"/>
+    <hyperlink ref="O34" r:id="rId26"/>
+    <hyperlink ref="O35" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
   <tableParts count="1">
-    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId29"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3019: Migrate related solution field.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$38</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="92">
   <si>
     <t>No</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>project with discussions having replies with files</t>
+  </si>
+  <si>
+    <t>asset_release with relations</t>
+  </si>
+  <si>
+    <t>related by 55844 as Translation</t>
+  </si>
+  <si>
+    <t>related by 55844 as Related Asset</t>
   </si>
 </sst>
 </file>
@@ -448,7 +457,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="129">
+  <cellStyleXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -496,6 +505,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -648,7 +660,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="129">
+  <cellStyles count="132">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -753,6 +765,9 @@
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -780,52 +795,6 @@
     <cellStyle name="Normale 2" xfId="1"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1074,6 +1043,52 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -1090,31 +1105,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S35" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:S35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S38" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S38"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="20" name="Type of content item" dataDxfId="20"/>
-    <tableColumn id="18" name="Nid" dataDxfId="0" dataCellStyle="Normale 2"/>
-    <tableColumn id="1" name="Title of content item" dataDxfId="19"/>
-    <tableColumn id="10" name="Collection_Name" dataDxfId="18"/>
-    <tableColumn id="3" name="Policy domain 1" dataDxfId="17"/>
-    <tableColumn id="27" name="Policy domain 2" dataDxfId="16" dataCellStyle="Normale 2"/>
-    <tableColumn id="22" name="New collection" dataDxfId="15"/>
-    <tableColumn id="30" name="Migrate" dataDxfId="14" dataCellStyle="Normale 2"/>
-    <tableColumn id="12" name="Abstract" dataDxfId="13"/>
-    <tableColumn id="8" name="Logo" dataDxfId="12"/>
-    <tableColumn id="2" name="Banner" dataDxfId="11"/>
-    <tableColumn id="15" name="Owner" dataDxfId="10"/>
-    <tableColumn id="5" name="Owner name" dataDxfId="9" dataCellStyle="Normale 2"/>
-    <tableColumn id="4" name="Owner type" dataDxfId="8" dataCellStyle="Normale 2"/>
-    <tableColumn id="9" name="Collection Owner" dataDxfId="7" dataCellStyle="Normale 2"/>
-    <tableColumn id="25" name="Elibrary Creation" dataDxfId="6"/>
-    <tableColumn id="26" name="Pre Moderation" dataDxfId="5"/>
-    <tableColumn id="13" name="Collection state" dataDxfId="4"/>
-    <tableColumn id="28" name="Content item state" dataDxfId="3" dataCellStyle="Normale 2"/>
+    <tableColumn id="20" name="Type of content item" dataDxfId="18"/>
+    <tableColumn id="18" name="Nid" dataDxfId="17" dataCellStyle="Normale 2"/>
+    <tableColumn id="1" name="Title of content item" dataDxfId="16"/>
+    <tableColumn id="10" name="Collection_Name" dataDxfId="15"/>
+    <tableColumn id="3" name="Policy domain 1" dataDxfId="14"/>
+    <tableColumn id="27" name="Policy domain 2" dataDxfId="13" dataCellStyle="Normale 2"/>
+    <tableColumn id="22" name="New collection" dataDxfId="12"/>
+    <tableColumn id="30" name="Migrate" dataDxfId="11" dataCellStyle="Normale 2"/>
+    <tableColumn id="12" name="Abstract" dataDxfId="10"/>
+    <tableColumn id="8" name="Logo" dataDxfId="9"/>
+    <tableColumn id="2" name="Banner" dataDxfId="8"/>
+    <tableColumn id="15" name="Owner" dataDxfId="7"/>
+    <tableColumn id="5" name="Owner name" dataDxfId="6" dataCellStyle="Normale 2"/>
+    <tableColumn id="4" name="Owner type" dataDxfId="5" dataCellStyle="Normale 2"/>
+    <tableColumn id="9" name="Collection Owner" dataDxfId="4" dataCellStyle="Normale 2"/>
+    <tableColumn id="25" name="Elibrary Creation" dataDxfId="3"/>
+    <tableColumn id="26" name="Pre Moderation" dataDxfId="2"/>
+    <tableColumn id="13" name="Collection state" dataDxfId="1"/>
+    <tableColumn id="28" name="Content item state" dataDxfId="0" dataCellStyle="Normale 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1386,7 +1401,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2473,7 +2488,9 @@
       </c>
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
+      <c r="R28" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="S28" s="12"/>
     </row>
     <row r="29" spans="1:19" ht="15" x14ac:dyDescent="0.2">
@@ -2511,7 +2528,9 @@
       </c>
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
+      <c r="R29" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="S29" s="12"/>
     </row>
     <row r="30" spans="1:19" ht="15" x14ac:dyDescent="0.2">
@@ -2547,7 +2566,9 @@
       </c>
       <c r="P30" s="10"/>
       <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
+      <c r="R30" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="S30" s="12"/>
     </row>
     <row r="31" spans="1:19" ht="15" x14ac:dyDescent="0.2">
@@ -2587,7 +2608,9 @@
       </c>
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
-      <c r="R31" s="10"/>
+      <c r="R31" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="S31" s="12"/>
     </row>
     <row r="32" spans="1:19" ht="15" x14ac:dyDescent="0.2">
@@ -2623,7 +2646,9 @@
       </c>
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
-      <c r="R32" s="10"/>
+      <c r="R32" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="S32" s="12"/>
     </row>
     <row r="33" spans="1:19" ht="15" x14ac:dyDescent="0.2">
@@ -2659,7 +2684,9 @@
       </c>
       <c r="P33" s="10"/>
       <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
+      <c r="R33" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="S33" s="12"/>
     </row>
     <row r="34" spans="1:19" ht="15" x14ac:dyDescent="0.2">
@@ -2695,7 +2722,9 @@
       </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
+      <c r="R34" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="S34" s="12"/>
     </row>
     <row r="35" spans="1:19" ht="15" x14ac:dyDescent="0.2">
@@ -2731,8 +2760,124 @@
       </c>
       <c r="P35" s="10"/>
       <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
+      <c r="R35" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="S35" s="12"/>
+    </row>
+    <row r="36" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="15">
+        <v>59180</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="S36" s="12"/>
+    </row>
+    <row r="37" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="15">
+        <v>59183</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="S37" s="12"/>
+    </row>
+    <row r="38" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="15">
+        <v>60208</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="S38" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2763,11 +2908,14 @@
     <hyperlink ref="O33" r:id="rId25"/>
     <hyperlink ref="O34" r:id="rId26"/>
     <hyperlink ref="O35" r:id="rId27"/>
+    <hyperlink ref="O36" r:id="rId28"/>
+    <hyperlink ref="O37" r:id="rId29"/>
+    <hyperlink ref="O38" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId32"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3060: Don't allow duplicates in 'owner_text'.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="92">
   <si>
     <t>No</t>
   </si>
@@ -457,7 +457,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="132">
+  <cellStyleXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -505,6 +505,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -660,7 +662,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="132">
+  <cellStyles count="134">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -768,6 +770,8 @@
     <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1902,8 +1906,7 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
+      <c r="N13" s="16"/>
       <c r="O13" s="13" t="s">
         <v>35</v>
       </c>
@@ -2753,8 +2756,12 @@
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
+      <c r="M35" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N35" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="O35" s="13" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
ISAICP-3408: Add Excel files version v1.16.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
+    <sheet name="5. Collections" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$34</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="91">
   <si>
     <t>No</t>
   </si>
@@ -107,18 +108,12 @@
     <t>Project</t>
   </si>
   <si>
-    <t>Invalid "New collection" cell</t>
-  </si>
-  <si>
     <t>Community</t>
   </si>
   <si>
     <t>Repository</t>
   </si>
   <si>
-    <t>Invalid collection name '#N/A'</t>
-  </si>
-  <si>
     <t>eProcurement</t>
   </si>
   <si>
@@ -128,18 +123,9 @@
     <t>project_project as solution in new collection</t>
   </si>
   <si>
-    <t>More than one Community or Repository</t>
-  </si>
-  <si>
-    <t>No Repository or Community</t>
-  </si>
-  <si>
     <t>Collection Owner</t>
   </si>
   <si>
-    <t>joeroe@example.com</t>
-  </si>
-  <si>
     <t>doe@example.com</t>
   </si>
   <si>
@@ -309,6 +295,18 @@
   </si>
   <si>
     <t>related by 55844 as Related Asset</t>
+  </si>
+  <si>
+    <t>Collection_name</t>
+  </si>
+  <si>
+    <t>eGovernment</t>
+  </si>
+  <si>
+    <t>Inexistent collection</t>
+  </si>
+  <si>
+    <t>Collection with errorneous items</t>
   </si>
 </sst>
 </file>
@@ -379,7 +377,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,8 +402,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -456,8 +466,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="134">
+  <cellStyleXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -592,8 +615,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -661,8 +686,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="134">
+  <cellStyles count="136">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -772,6 +819,8 @@
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1109,8 +1158,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S38" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:S38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S34" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S34"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1405,7 +1454,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1415,8 +1464,8 @@
   <cols>
     <col min="1" max="1" width="19.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="38" style="8" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.5" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
@@ -1426,11 +1475,11 @@
     <col min="12" max="12" width="9" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.83203125" style="8" customWidth="1"/>
     <col min="14" max="14" width="18.5" style="8" customWidth="1"/>
-    <col min="15" max="15" width="21.1640625" style="8" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="24.1640625" style="8"/>
   </cols>
   <sheetData>
@@ -1439,7 +1488,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
@@ -1472,13 +1521,13 @@
         <v>6</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>5</v>
@@ -1487,10 +1536,10 @@
         <v>4</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -1504,7 +1553,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>3</v>
@@ -1527,14 +1576,14 @@
         <v>18</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>16</v>
@@ -1561,7 +1610,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="8" t="s">
@@ -1582,7 +1631,7 @@
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="S4" s="12"/>
     </row>
@@ -1597,7 +1646,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="8" t="s">
@@ -1625,20 +1674,17 @@
         <v>1</v>
       </c>
       <c r="B6" s="9">
-        <v>58729</v>
+        <v>60736</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="8" t="e">
-        <v>#N/A</v>
+        <v>19</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>16</v>
@@ -1654,101 +1700,124 @@
       <c r="R6" s="10"/>
       <c r="S6" s="12"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="9">
-        <v>60736</v>
+        <v>58694</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="E7" s="10"/>
-      <c r="F7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>16</v>
+      <c r="F7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
+      <c r="O7" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
       <c r="S7" s="12"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="9">
-        <v>156207</v>
+        <v>49860</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="10" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>16</v>
+      <c r="F8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="10"/>
+      <c r="L8" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
-      <c r="S8" s="12"/>
+      <c r="S8" s="17" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="9">
-        <v>145807</v>
+        <v>87737</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="8" t="s">
-        <v>3</v>
+      <c r="F9" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
+      <c r="N9" s="16"/>
       <c r="O9" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
@@ -1757,26 +1826,29 @@
     </row>
     <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B10" s="9">
-        <v>105945</v>
+        <v>139528</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="14" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>16</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -1784,29 +1856,31 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
-      <c r="S10" s="12"/>
+      <c r="S10" s="17" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B11" s="9">
-        <v>58694</v>
+        <v>42233</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>16</v>
@@ -1815,7 +1889,7 @@
         <v>16</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -1823,7 +1897,7 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
@@ -1832,67 +1906,59 @@
     </row>
     <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B12" s="9">
-        <v>49860</v>
+        <v>138766</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H12" s="15" t="s">
         <v>16</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N12" s="16" t="s">
-        <v>82</v>
-      </c>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
       <c r="O12" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
-      <c r="S12" s="17" t="s">
-        <v>71</v>
-      </c>
+      <c r="S12" s="12"/>
     </row>
     <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B13" s="9">
-        <v>87737</v>
+        <v>133560</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>16</v>
@@ -1901,14 +1967,15 @@
         <v>16</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
-      <c r="N13" s="16"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
       <c r="O13" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
@@ -1916,21 +1983,21 @@
       <c r="S13" s="12"/>
     </row>
     <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>38</v>
+      <c r="A14" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="B14" s="9">
-        <v>139528</v>
+        <v>53012</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>16</v>
@@ -1939,7 +2006,7 @@
         <v>16</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -1947,31 +2014,29 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="17" t="s">
-        <v>72</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="19"/>
     </row>
     <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="9">
-        <v>42233</v>
+        <v>63578</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>16</v>
@@ -1980,7 +2045,7 @@
         <v>16</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -1988,7 +2053,7 @@
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
@@ -2000,17 +2065,17 @@
         <v>38</v>
       </c>
       <c r="B16" s="9">
-        <v>138766</v>
+        <v>155691</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>16</v>
@@ -2019,7 +2084,7 @@
         <v>16</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -2027,7 +2092,7 @@
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
@@ -2039,7 +2104,7 @@
         <v>45</v>
       </c>
       <c r="B17" s="9">
-        <v>133560</v>
+        <v>27607</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>46</v>
@@ -2049,7 +2114,7 @@
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>16</v>
@@ -2058,7 +2123,7 @@
         <v>16</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
@@ -2066,29 +2131,31 @@
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
-      <c r="S17" s="12"/>
+      <c r="S17" s="17" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="18" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
-        <v>39</v>
+      <c r="A18" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="B18" s="9">
-        <v>53012</v>
+        <v>155894</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>16</v>
@@ -2097,7 +2164,7 @@
         <v>16</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -2105,29 +2172,29 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="19"/>
+        <v>30</v>
+      </c>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="12"/>
     </row>
     <row r="19" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B19" s="9">
-        <v>63578</v>
+        <v>152066</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>16</v>
@@ -2136,7 +2203,7 @@
         <v>16</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -2144,7 +2211,7 @@
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
@@ -2153,20 +2220,20 @@
     </row>
     <row r="20" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B20" s="9">
-        <v>155691</v>
+        <v>145278</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>16</v>
@@ -2175,7 +2242,7 @@
         <v>16</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
@@ -2183,7 +2250,7 @@
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
@@ -2192,78 +2259,70 @@
     </row>
     <row r="21" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B21" s="9">
-        <v>27607</v>
-      </c>
-      <c r="C21" s="10" t="s">
+        <v>59642</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="E21" s="10"/>
-      <c r="F21" s="14" t="s">
-        <v>28</v>
+      <c r="F21" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H21" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
-      <c r="O21" s="13" t="s">
-        <v>35</v>
+      <c r="O21" s="22" t="s">
+        <v>53</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
-      <c r="S21" s="17" t="s">
-        <v>73</v>
-      </c>
+      <c r="S21" s="12"/>
     </row>
     <row r="22" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="B22" s="9">
-        <v>155894</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>52</v>
+        <v>149141</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>54</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="E22" s="10"/>
-      <c r="F22" s="14" t="s">
-        <v>28</v>
+      <c r="F22" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H22" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
-      <c r="O22" s="13" t="s">
-        <v>35</v>
+      <c r="O22" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
@@ -2272,29 +2331,26 @@
     </row>
     <row r="23" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="B23" s="9">
-        <v>152066</v>
+        <v>144326</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>9</v>
+        <v>63</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="14" t="s">
-        <v>28</v>
+      <c r="F23" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H23" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -2302,38 +2358,37 @@
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
+      <c r="R23" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="S23" s="12"/>
     </row>
     <row r="24" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="B24" s="9">
-        <v>145278</v>
+        <v>76726</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>9</v>
+        <v>65</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="F24" s="14" t="s">
-        <v>28</v>
+      <c r="F24" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H24" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -2341,29 +2396,31 @@
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
+      <c r="R24" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="S24" s="12"/>
     </row>
     <row r="25" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B25" s="9">
-        <v>59642</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>60</v>
+        <v>102713</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>0</v>
@@ -2376,30 +2433,32 @@
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
-      <c r="O25" s="22" t="s">
-        <v>58</v>
+      <c r="O25" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
+      <c r="R25" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="S25" s="12"/>
     </row>
     <row r="26" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B26" s="9">
-        <v>149141</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>61</v>
+        <v>125548</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="20" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>0</v>
@@ -2412,30 +2471,32 @@
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
-      <c r="O26" s="22" t="s">
-        <v>63</v>
+      <c r="O26" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
+      <c r="R26" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="S26" s="12"/>
     </row>
     <row r="27" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" s="9">
-        <v>144326</v>
+        <v>42444</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>0</v>
@@ -2445,35 +2506,41 @@
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
+      <c r="L27" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N27" s="16" t="s">
+        <v>78</v>
+      </c>
       <c r="O27" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
       <c r="R27" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S27" s="12"/>
     </row>
     <row r="28" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B28" s="9">
-        <v>76726</v>
+        <v>150255</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>0</v>
@@ -2487,31 +2554,31 @@
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
       <c r="R28" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S28" s="12"/>
     </row>
     <row r="29" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="B29" s="9">
-        <v>102713</v>
+        <v>65803</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>74</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>0</v>
@@ -2521,37 +2588,35 @@
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
-      <c r="L29" s="10" t="s">
-        <v>87</v>
-      </c>
+      <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
       <c r="R29" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S29" s="12"/>
     </row>
     <row r="30" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B30" s="9">
-        <v>125548</v>
+        <v>156973</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>0</v>
@@ -2565,12 +2630,12 @@
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
       <c r="O30" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P30" s="10"/>
       <c r="Q30" s="10"/>
       <c r="R30" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S30" s="12"/>
     </row>
@@ -2579,17 +2644,17 @@
         <v>23</v>
       </c>
       <c r="B31" s="9">
-        <v>42444</v>
+        <v>63567</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>0</v>
@@ -2600,38 +2665,38 @@
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
-      <c r="M31" s="10" t="s">
-        <v>85</v>
+      <c r="M31" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="N31" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="O31" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
       <c r="R31" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S31" s="12"/>
     </row>
     <row r="32" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="9">
-        <v>150255</v>
+        <v>1</v>
+      </c>
+      <c r="B32" s="15">
+        <v>59180</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>0</v>
@@ -2645,31 +2710,31 @@
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
       <c r="O32" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
       <c r="R32" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S32" s="12"/>
     </row>
     <row r="33" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" s="9">
-        <v>65803</v>
+        <v>1</v>
+      </c>
+      <c r="B33" s="15">
+        <v>59183</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>0</v>
@@ -2683,31 +2748,31 @@
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
       <c r="O33" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P33" s="10"/>
       <c r="Q33" s="10"/>
       <c r="R33" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S33" s="12"/>
     </row>
     <row r="34" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" s="9">
-        <v>156973</v>
+        <v>1</v>
+      </c>
+      <c r="B34" s="15">
+        <v>60208</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>86</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>0</v>
@@ -2721,208 +2786,242 @@
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
       <c r="O34" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
       <c r="R34" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S34" s="12"/>
-    </row>
-    <row r="35" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="9">
-        <v>63567</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N35" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="O35" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="S35" s="12"/>
-    </row>
-    <row r="36" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="15">
-        <v>59180</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="S36" s="12"/>
-    </row>
-    <row r="37" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="15">
-        <v>59183</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H37" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="S37" s="12"/>
-    </row>
-    <row r="38" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="15">
-        <v>60208</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="S38" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O9" r:id="rId1"/>
-    <hyperlink ref="O11" r:id="rId2"/>
-    <hyperlink ref="O12" r:id="rId3"/>
+    <hyperlink ref="O7" r:id="rId1"/>
+    <hyperlink ref="O8" r:id="rId2"/>
+    <hyperlink ref="O9" r:id="rId3"/>
     <hyperlink ref="O10" r:id="rId4"/>
-    <hyperlink ref="O13" r:id="rId5"/>
-    <hyperlink ref="O14" r:id="rId6"/>
-    <hyperlink ref="O18" r:id="rId7"/>
-    <hyperlink ref="O19" r:id="rId8"/>
-    <hyperlink ref="O20" r:id="rId9"/>
-    <hyperlink ref="O17" r:id="rId10"/>
-    <hyperlink ref="O15" r:id="rId11"/>
-    <hyperlink ref="O16" r:id="rId12"/>
-    <hyperlink ref="O21" r:id="rId13"/>
-    <hyperlink ref="O22" r:id="rId14"/>
-    <hyperlink ref="O23" r:id="rId15"/>
-    <hyperlink ref="O24" r:id="rId16"/>
-    <hyperlink ref="O26" r:id="rId17"/>
-    <hyperlink ref="O25" r:id="rId18"/>
-    <hyperlink ref="O27" r:id="rId19"/>
-    <hyperlink ref="O28" r:id="rId20"/>
-    <hyperlink ref="O29" r:id="rId21"/>
-    <hyperlink ref="O30" r:id="rId22"/>
-    <hyperlink ref="O31" r:id="rId23"/>
-    <hyperlink ref="O32" r:id="rId24"/>
-    <hyperlink ref="O33" r:id="rId25"/>
-    <hyperlink ref="O34" r:id="rId26"/>
-    <hyperlink ref="O35" r:id="rId27"/>
-    <hyperlink ref="O36" r:id="rId28"/>
-    <hyperlink ref="O37" r:id="rId29"/>
-    <hyperlink ref="O38" r:id="rId30"/>
+    <hyperlink ref="O14" r:id="rId5"/>
+    <hyperlink ref="O15" r:id="rId6"/>
+    <hyperlink ref="O16" r:id="rId7"/>
+    <hyperlink ref="O13" r:id="rId8"/>
+    <hyperlink ref="O11" r:id="rId9"/>
+    <hyperlink ref="O12" r:id="rId10"/>
+    <hyperlink ref="O17" r:id="rId11"/>
+    <hyperlink ref="O18" r:id="rId12"/>
+    <hyperlink ref="O19" r:id="rId13"/>
+    <hyperlink ref="O20" r:id="rId14"/>
+    <hyperlink ref="O22" r:id="rId15"/>
+    <hyperlink ref="O21" r:id="rId16"/>
+    <hyperlink ref="O23" r:id="rId17"/>
+    <hyperlink ref="O24" r:id="rId18"/>
+    <hyperlink ref="O25" r:id="rId19"/>
+    <hyperlink ref="O26" r:id="rId20"/>
+    <hyperlink ref="O27" r:id="rId21"/>
+    <hyperlink ref="O28" r:id="rId22"/>
+    <hyperlink ref="O29" r:id="rId23"/>
+    <hyperlink ref="O30" r:id="rId24"/>
+    <hyperlink ref="O31" r:id="rId25"/>
+    <hyperlink ref="O32" r:id="rId26"/>
+    <hyperlink ref="O33" r:id="rId27"/>
+    <hyperlink ref="O34" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
   <tableParts count="1">
-    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId30"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="S1:AF6"/>
+  <sheetViews>
+    <sheetView topLeftCell="R1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5" customWidth="1"/>
+    <col min="19" max="19" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="19:32" x14ac:dyDescent="0.2">
+      <c r="S1" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="V1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="X1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z1" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF1" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="19:32" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T2" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="19:32" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="V3" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA3" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB3" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC3" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="19:32" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S4" s="30">
+        <v>59642</v>
+      </c>
+      <c r="T4" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="U4" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="V4" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="W4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="19:32" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S5" s="30">
+        <v>149141</v>
+      </c>
+      <c r="T5" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="U5" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="V5" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="W5" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="19:32" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S6" s="30">
+        <v>42444</v>
+      </c>
+      <c r="T6" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="U6" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="V6" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="W6" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB6" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC6" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF6" s="30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AC3" r:id="rId1"/>
+    <hyperlink ref="AC4" r:id="rId2"/>
+    <hyperlink ref="AC5" r:id="rId3"/>
+    <hyperlink ref="AC6" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-3408, ISAICP-3189: Not new collections data is migrated from Project, Community, Repository. Colelction owner is taken from the Excel file.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="96">
   <si>
     <t>No</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Collection Owner</t>
   </si>
   <si>
-    <t>doe@example.com</t>
-  </si>
-  <si>
     <t>Invalid</t>
   </si>
   <si>
@@ -195,24 +192,15 @@
     <t>Open government</t>
   </si>
   <si>
-    <t>baby.doe@example.com</t>
-  </si>
-  <si>
     <t>Community as base for collection</t>
   </si>
   <si>
-    <t>Collection from Repository</t>
-  </si>
-  <si>
     <t>Collection from Community</t>
   </si>
   <si>
     <t>Collaboration</t>
   </si>
   <si>
-    <t>jbloggs@example.com</t>
-  </si>
-  <si>
     <t>Abstract for a new collection</t>
   </si>
   <si>
@@ -306,7 +294,34 @@
     <t>Inexistent collection</t>
   </si>
   <si>
-    <t>Collection with errorneous items</t>
+    <t>Collection with invalid node</t>
+  </si>
+  <si>
+    <t>Project as base for collection</t>
+  </si>
+  <si>
+    <t>Collection from Project</t>
+  </si>
+  <si>
+    <t>joel@sambreville.be</t>
+  </si>
+  <si>
+    <t>viktor.hristov@hotmail.com</t>
+  </si>
+  <si>
+    <t>eric.smets@fks.be</t>
+  </si>
+  <si>
+    <t>mux2005@gmail.com</t>
+  </si>
+  <si>
+    <t>riccardo.sibilia@vtg.admin.ch</t>
+  </si>
+  <si>
+    <t>tbenita@atreal.fr, aanguix@gvsig.com</t>
+  </si>
+  <si>
+    <t>Collection with erroneous items</t>
   </si>
 </sst>
 </file>
@@ -415,7 +430,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -479,8 +494,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="136">
+  <cellStyleXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -527,7 +551,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -618,7 +648,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -651,13 +681,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -683,9 +707,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -698,18 +719,26 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="136">
+  <cellStyles count="142">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -732,6 +761,7 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
@@ -821,6 +851,12 @@
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -843,7 +879,6 @@
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="46" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="1"/>
   </cellStyles>
@@ -1464,7 +1499,7 @@
   <cols>
     <col min="1" max="1" width="19.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" style="8" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.5" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="8" bestFit="1" customWidth="1"/>
@@ -1473,9 +1508,9 @@
     <col min="10" max="10" width="7.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" style="8" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.1640625" style="8" customWidth="1"/>
     <col min="16" max="16" width="17.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.1640625" style="8" bestFit="1" customWidth="1"/>
@@ -1488,7 +1523,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
@@ -1521,10 +1556,10 @@
         <v>6</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>29</v>
@@ -1536,13 +1571,13 @@
         <v>4</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1553,7 +1588,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>3</v>
@@ -1564,8 +1599,11 @@
       <c r="H2" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O2" s="22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1576,14 +1614,14 @@
         <v>18</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>16</v>
@@ -1593,13 +1631,15 @@
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
-      <c r="O3" s="11"/>
+      <c r="O3" s="22" t="s">
+        <v>93</v>
+      </c>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
-      <c r="S3" s="12"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S3" s="11"/>
+    </row>
+    <row r="4" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
@@ -1610,7 +1650,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="8" t="s">
@@ -1627,15 +1667,17 @@
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
+      <c r="O4" s="22" t="s">
+        <v>93</v>
+      </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="S4" s="12"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="S4" s="11"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
@@ -1646,7 +1688,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="8" t="s">
@@ -1663,11 +1705,13 @@
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="O5" s="22" t="s">
+        <v>93</v>
+      </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
-      <c r="S5" s="12"/>
+      <c r="S5" s="11"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
@@ -1698,9 +1742,9 @@
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
-      <c r="S6" s="12"/>
-    </row>
-    <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S6" s="11"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>1</v>
       </c>
@@ -1714,30 +1758,30 @@
         <v>9</v>
       </c>
       <c r="E7" s="10"/>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
-      <c r="O7" s="13" t="s">
-        <v>30</v>
+      <c r="O7" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
-      <c r="S7" s="12"/>
+      <c r="S7" s="11"/>
     </row>
     <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -1753,40 +1797,40 @@
         <v>9</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>30</v>
+        <v>75</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
-      <c r="S8" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S8" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
@@ -1794,580 +1838,590 @@
         <v>87737</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="13" t="s">
-        <v>30</v>
+      <c r="N9" s="14"/>
+      <c r="O9" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
-      <c r="S9" s="12"/>
+      <c r="S9" s="11"/>
     </row>
     <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="9">
         <v>139528</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="10"/>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="13" t="s">
-        <v>30</v>
+      <c r="O10" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
-      <c r="S10" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S10" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="9">
         <v>42233</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="10"/>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="13" t="s">
-        <v>30</v>
+      <c r="O11" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
-      <c r="S11" s="12"/>
-    </row>
-    <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S11" s="11"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="9">
         <v>138766</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="13" t="s">
-        <v>30</v>
+      <c r="O12" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
-      <c r="S12" s="12"/>
-    </row>
-    <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S12" s="11"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="9">
         <v>133560</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="10"/>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="13" t="s">
-        <v>30</v>
+      <c r="O13" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
-      <c r="S13" s="12"/>
-    </row>
-    <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>34</v>
+      <c r="S13" s="11"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="B14" s="9">
         <v>53012</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="10"/>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
-      <c r="O14" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="19"/>
-    </row>
-    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="O14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="17"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="9">
         <v>63578</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
-      <c r="O15" s="13" t="s">
-        <v>30</v>
+      <c r="O15" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
-      <c r="S15" s="12"/>
-    </row>
-    <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S15" s="11"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="9">
         <v>155691</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
-      <c r="O16" s="13" t="s">
-        <v>30</v>
+      <c r="O16" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
-      <c r="S16" s="12"/>
+      <c r="S16" s="11"/>
     </row>
     <row r="17" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="9">
         <v>27607</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="10"/>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
-      <c r="O17" s="13" t="s">
-        <v>30</v>
+      <c r="O17" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
-      <c r="S17" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S17" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="9">
         <v>155894</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
-      <c r="O18" s="13" t="s">
-        <v>30</v>
+      <c r="O18" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
-      <c r="S18" s="12"/>
-    </row>
-    <row r="19" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S18" s="11"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="9">
         <v>152066</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="10"/>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H19" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
-      <c r="O19" s="13" t="s">
-        <v>30</v>
+      <c r="O19" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
-      <c r="S19" s="12"/>
-    </row>
-    <row r="20" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S19" s="11"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="9">
         <v>145278</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
-      <c r="O20" s="13" t="s">
-        <v>30</v>
+      <c r="O20" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
-      <c r="S20" s="12"/>
-    </row>
-    <row r="21" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S20" s="11"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" s="9">
-        <v>59642</v>
-      </c>
-      <c r="C21" s="21" t="s">
+        <v>42438</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="18" t="s">
         <v>51</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="20" t="s">
-        <v>52</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="22" t="s">
-        <v>53</v>
+      <c r="L21" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
-      <c r="S21" s="12"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S21" s="11"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="9">
         <v>149141</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="18" t="s">
         <v>54</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="20" t="s">
-        <v>57</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
+      <c r="L22" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
-      <c r="O22" s="22" t="s">
-        <v>58</v>
+      <c r="O22" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
-      <c r="S22" s="12"/>
-    </row>
-    <row r="23" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S22" s="11"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" s="9">
-        <v>144326</v>
+        <v>82307</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="20" t="s">
-        <v>52</v>
+      <c r="F23" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
+      <c r="L23" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
-      <c r="O23" s="13" t="s">
-        <v>30</v>
+      <c r="O23" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
       <c r="R23" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S23" s="12"/>
-    </row>
-    <row r="24" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="S23" s="11"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>1</v>
       </c>
@@ -2375,19 +2429,19 @@
         <v>76726</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="F24" s="20" t="s">
-        <v>52</v>
+      <c r="F24" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H24" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J24" s="10"/>
@@ -2395,17 +2449,17 @@
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
-      <c r="O24" s="13" t="s">
-        <v>30</v>
+      <c r="O24" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
       <c r="R24" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S24" s="12"/>
-    </row>
-    <row r="25" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="S24" s="11"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>1</v>
       </c>
@@ -2413,57 +2467,57 @@
         <v>102713</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E25" s="10"/>
-      <c r="F25" s="20" t="s">
-        <v>52</v>
+      <c r="F25" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="13" t="s">
-        <v>30</v>
+      <c r="N25" s="14"/>
+      <c r="O25" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S25" s="12"/>
-    </row>
-    <row r="26" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="S25" s="11"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="9">
         <v>125548</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E26" s="10"/>
-      <c r="F26" s="20" t="s">
-        <v>52</v>
+      <c r="F26" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="H26" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J26" s="10"/>
@@ -2471,17 +2525,17 @@
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
-      <c r="O26" s="13" t="s">
-        <v>30</v>
+      <c r="O26" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
       <c r="R26" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S26" s="12"/>
-    </row>
-    <row r="27" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="S26" s="11"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>23</v>
       </c>
@@ -2489,63 +2543,61 @@
         <v>42444</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E27" s="10"/>
-      <c r="F27" s="20" t="s">
-        <v>52</v>
+      <c r="F27" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H27" s="15" t="s">
+      <c r="H27" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
-      <c r="L27" s="10" t="s">
-        <v>82</v>
-      </c>
+      <c r="L27" s="10"/>
       <c r="M27" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="N27" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="O27" s="13" t="s">
-        <v>30</v>
+        <v>76</v>
+      </c>
+      <c r="N27" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="O27" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
       <c r="R27" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S27" s="12"/>
-    </row>
-    <row r="28" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="S27" s="11"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="9">
         <v>150255</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E28" s="10"/>
-      <c r="F28" s="20" t="s">
-        <v>52</v>
+      <c r="F28" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J28" s="10"/>
@@ -2553,37 +2605,37 @@
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="13" t="s">
-        <v>30</v>
+      <c r="O28" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
       <c r="R28" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S28" s="12"/>
-    </row>
-    <row r="29" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="S28" s="11"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="9">
         <v>65803</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E29" s="10"/>
-      <c r="F29" s="20" t="s">
-        <v>52</v>
+      <c r="F29" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="H29" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J29" s="10"/>
@@ -2591,37 +2643,37 @@
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
-      <c r="O29" s="13" t="s">
-        <v>30</v>
+      <c r="O29" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
       <c r="R29" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S29" s="12"/>
-    </row>
-    <row r="30" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="S29" s="11"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="9">
         <v>156973</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E30" s="10"/>
-      <c r="F30" s="20" t="s">
-        <v>52</v>
+      <c r="F30" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J30" s="10"/>
@@ -2629,17 +2681,17 @@
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
-      <c r="O30" s="13" t="s">
-        <v>30</v>
+      <c r="O30" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P30" s="10"/>
       <c r="Q30" s="10"/>
       <c r="R30" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S30" s="12"/>
-    </row>
-    <row r="31" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="S30" s="11"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>23</v>
       </c>
@@ -2647,61 +2699,61 @@
         <v>63567</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E31" s="10"/>
-      <c r="F31" s="20" t="s">
-        <v>52</v>
+      <c r="F31" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H31" s="15" t="s">
+      <c r="H31" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
       <c r="M31" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="N31" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="O31" s="13" t="s">
-        <v>30</v>
+        <v>75</v>
+      </c>
+      <c r="N31" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="O31" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
       <c r="R31" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S31" s="12"/>
-    </row>
-    <row r="32" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="S31" s="11"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="13">
         <v>59180</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E32" s="10"/>
-      <c r="F32" s="20" t="s">
-        <v>52</v>
+      <c r="F32" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="H32" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J32" s="10"/>
@@ -2709,37 +2761,37 @@
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
-      <c r="O32" s="13" t="s">
-        <v>30</v>
+      <c r="O32" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
       <c r="R32" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S32" s="12"/>
-    </row>
-    <row r="33" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="S32" s="11"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="13">
         <v>59183</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E33" s="10"/>
-      <c r="F33" s="20" t="s">
-        <v>52</v>
+      <c r="F33" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H33" s="15" t="s">
+      <c r="H33" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J33" s="10"/>
@@ -2747,37 +2799,37 @@
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
-      <c r="O33" s="13" t="s">
-        <v>30</v>
+      <c r="O33" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P33" s="10"/>
       <c r="Q33" s="10"/>
       <c r="R33" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S33" s="12"/>
-    </row>
-    <row r="34" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="S33" s="11"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="13">
         <v>60208</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E34" s="10"/>
-      <c r="F34" s="20" t="s">
-        <v>52</v>
+      <c r="F34" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H34" s="15" t="s">
+      <c r="H34" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J34" s="10"/>
@@ -2785,58 +2837,36 @@
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
-      <c r="O34" s="13" t="s">
-        <v>30</v>
+      <c r="O34" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
       <c r="R34" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S34" s="12"/>
+        <v>60</v>
+      </c>
+      <c r="S34" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O7" r:id="rId1"/>
-    <hyperlink ref="O8" r:id="rId2"/>
-    <hyperlink ref="O9" r:id="rId3"/>
-    <hyperlink ref="O10" r:id="rId4"/>
-    <hyperlink ref="O14" r:id="rId5"/>
-    <hyperlink ref="O15" r:id="rId6"/>
-    <hyperlink ref="O16" r:id="rId7"/>
-    <hyperlink ref="O13" r:id="rId8"/>
-    <hyperlink ref="O11" r:id="rId9"/>
-    <hyperlink ref="O12" r:id="rId10"/>
-    <hyperlink ref="O17" r:id="rId11"/>
-    <hyperlink ref="O18" r:id="rId12"/>
-    <hyperlink ref="O19" r:id="rId13"/>
-    <hyperlink ref="O20" r:id="rId14"/>
-    <hyperlink ref="O22" r:id="rId15"/>
-    <hyperlink ref="O21" r:id="rId16"/>
-    <hyperlink ref="O23" r:id="rId17"/>
-    <hyperlink ref="O24" r:id="rId18"/>
-    <hyperlink ref="O25" r:id="rId19"/>
-    <hyperlink ref="O26" r:id="rId20"/>
-    <hyperlink ref="O27" r:id="rId21"/>
-    <hyperlink ref="O28" r:id="rId22"/>
-    <hyperlink ref="O29" r:id="rId23"/>
-    <hyperlink ref="O30" r:id="rId24"/>
-    <hyperlink ref="O31" r:id="rId25"/>
-    <hyperlink ref="O32" r:id="rId26"/>
-    <hyperlink ref="O33" r:id="rId27"/>
-    <hyperlink ref="O34" r:id="rId28"/>
+    <hyperlink ref="O7" r:id="rId1" display="doe@example.com"/>
+    <hyperlink ref="O21" r:id="rId2" display="baby.doe@example.com"/>
+    <hyperlink ref="O23" r:id="rId3" display="doe@example.com"/>
+    <hyperlink ref="O8:O19" r:id="rId4" display="doe@example.com"/>
+    <hyperlink ref="O20" r:id="rId5" display="doe@example.com"/>
+    <hyperlink ref="O24:O34" r:id="rId6" display="doe@example.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="S1:AF6"/>
+  <dimension ref="S1:AF7"/>
   <sheetViews>
     <sheetView topLeftCell="R1" zoomScale="163" workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
@@ -2846,7 +2876,7 @@
   <cols>
     <col min="1" max="17" width="0" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="7.5" customWidth="1"/>
-    <col min="19" max="19" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
@@ -2856,172 +2886,196 @@
     <col min="26" max="26" width="6.5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="38.83203125" customWidth="1"/>
     <col min="30" max="30" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="19:32" x14ac:dyDescent="0.2">
-      <c r="S1" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="T1" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="U1" s="24" t="s">
+      <c r="S1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="U1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="24" t="s">
+      <c r="V1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="24" t="s">
+      <c r="W1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="24" t="s">
+      <c r="X1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" s="24" t="s">
+      <c r="Y1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="24" t="s">
+      <c r="Z1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="24" t="s">
+      <c r="AA1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="19:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T2" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC2" s="22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="19:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="V3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA3" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" s="24" t="s">
+      <c r="AB3" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="19:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S4" s="28">
+        <v>42438</v>
+      </c>
+      <c r="T4" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="U4" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="V4" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="W4" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB4" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="19:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S5" s="26">
+        <v>149141</v>
+      </c>
+      <c r="T5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="V5" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="W5" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="19:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S6" s="28">
+        <v>82307</v>
+      </c>
+      <c r="T6" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="U6" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="V6" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="W6" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="AC1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD1" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE1" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF1" s="24" t="s">
+      <c r="AB6" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF6" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="19:32" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="T2" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="U2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="V2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="W2" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="19:32" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="T3" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="U3" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="V3" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="W3" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="X3" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA3" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB3" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC3" s="29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="19:32" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="S4" s="30">
-        <v>59642</v>
-      </c>
-      <c r="T4" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="U4" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="V4" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="W4" s="25" t="s">
+    <row r="7" spans="19:32" x14ac:dyDescent="0.2">
+      <c r="S7" s="29">
+        <v>9999999</v>
+      </c>
+      <c r="T7" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="U7" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="V7" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="W7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AC4" s="32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="19:32" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="S5" s="30">
-        <v>149141</v>
-      </c>
-      <c r="T5" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="U5" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="V5" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="W5" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="32" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="19:32" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="S6" s="30">
-        <v>42444</v>
-      </c>
-      <c r="T6" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="U6" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="V6" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="W6" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB6" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC6" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF6" s="30" t="s">
-        <v>64</v>
+      <c r="AC7" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="AC3" r:id="rId1"/>
-    <hyperlink ref="AC4" r:id="rId2"/>
-    <hyperlink ref="AC5" r:id="rId3"/>
-    <hyperlink ref="AC6" r:id="rId4"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISAICP-2972: Add news test cases for Custom Pages.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -16,7 +16,7 @@
     <sheet name="5. Collections" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$37</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="103">
   <si>
     <t>No</t>
   </si>
@@ -322,6 +322,27 @@
   </si>
   <si>
     <t>Collection with erroneous items</t>
+  </si>
+  <si>
+    <t>Community with custom section</t>
+  </si>
+  <si>
+    <t>john.doe@example.com</t>
+  </si>
+  <si>
+    <t>Collection with 2 entities having custom section</t>
+  </si>
+  <si>
+    <t>Project with custom section</t>
+  </si>
+  <si>
+    <t>Collection with 1 entity having custom section</t>
+  </si>
+  <si>
+    <t>jane.roe@example.com</t>
+  </si>
+  <si>
+    <t>Community with 2 custom sections</t>
   </si>
 </sst>
 </file>
@@ -430,7 +451,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -503,8 +524,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="142">
+  <cellStyleXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -647,8 +679,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -737,8 +779,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="142">
+  <cellStyles count="152">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -857,6 +908,16 @@
     <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1193,8 +1254,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S34" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:S34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S37" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S37"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1489,7 +1550,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1500,7 +1561,7 @@
     <col min="1" max="1" width="19.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.1640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.5" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
@@ -2847,6 +2908,118 @@
       </c>
       <c r="S34" s="11"/>
     </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="13">
+        <v>157710</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="M35" s="34"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="11"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="13">
+        <v>27024</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="11"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="13">
+        <v>26768</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="M37" s="34"/>
+      <c r="N37" s="34"/>
+      <c r="O37" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="11"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O7" r:id="rId1" display="doe@example.com"/>
@@ -2866,7 +3039,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="S1:AF7"/>
+  <dimension ref="S1:AF9"/>
   <sheetViews>
     <sheetView topLeftCell="R1" zoomScale="163" workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
@@ -2877,7 +3050,7 @@
     <col min="1" max="17" width="0" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="7.5" customWidth="1"/>
     <col min="19" max="19" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -3074,6 +3247,46 @@
         <v>92</v>
       </c>
     </row>
+    <row r="8" spans="19:32" x14ac:dyDescent="0.2">
+      <c r="S8" s="28">
+        <v>157710</v>
+      </c>
+      <c r="T8" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="U8" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="V8" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="W8" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="19:32" x14ac:dyDescent="0.2">
+      <c r="S9" s="32">
+        <v>26768</v>
+      </c>
+      <c r="T9" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="U9" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="V9" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="W9" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="32" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
ISAICP-3443: Foundation for centralising file migration. Only attachments were added now.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -2987,7 +2987,7 @@
         <v>24</v>
       </c>
       <c r="B37" s="13">
-        <v>26768</v>
+        <v>66790</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>96</v>
@@ -3269,7 +3269,7 @@
     </row>
     <row r="9" spans="19:32" x14ac:dyDescent="0.2">
       <c r="S9" s="32">
-        <v>26768</v>
+        <v>66790</v>
       </c>
       <c r="T9" s="33" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
Switch to version v1.18 of the Excel file.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
@@ -1552,7 +1552,7 @@
   </sheetPr>
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3039,251 +3039,249 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="S1:AF9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="36.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="17" width="0" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="7.5" customWidth="1"/>
-    <col min="19" max="19" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="38.83203125" customWidth="1"/>
-    <col min="30" max="30" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="19:32" x14ac:dyDescent="0.2">
-      <c r="S1" s="20" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="B1" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="C1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AC1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="AE1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="AF1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="19:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="T2" s="31" t="s">
+    <row r="2" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="U2" s="23" t="s">
+      <c r="C2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="23" t="s">
+      <c r="D2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="W2" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC2" s="22" t="s">
+      <c r="E2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="22" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="19:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="T3" s="23" t="s">
+    <row r="3" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="22" t="s">
+      <c r="C3" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="V3" s="24" t="s">
+      <c r="D3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="W3" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="X3" s="23" t="s">
+      <c r="E3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="AA3" s="23" t="s">
+      <c r="I3" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="AB3" s="25" t="s">
+      <c r="J3" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="K3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="19:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="S4" s="28">
+    <row r="4" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28">
         <v>42438</v>
       </c>
-      <c r="T4" s="23" t="s">
+      <c r="B4" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="U4" s="22" t="s">
+      <c r="C4" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="V4" s="27" t="s">
+      <c r="D4" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="W4" s="22" t="s">
+      <c r="E4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AA4" s="28" t="s">
+      <c r="I4" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="AB4" s="28" t="s">
+      <c r="J4" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="K4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="19:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="S5" s="26">
+    <row r="5" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="26">
         <v>149141</v>
       </c>
-      <c r="T5" s="23" t="s">
+      <c r="B5" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="U5" s="22" t="s">
+      <c r="C5" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="V5" s="27" t="s">
+      <c r="D5" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="W5" s="22" t="s">
+      <c r="E5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="K5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="19:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="S6" s="28">
+    <row r="6" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="28">
         <v>82307</v>
       </c>
-      <c r="T6" s="26" t="s">
+      <c r="B6" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="U6" s="22" t="s">
+      <c r="C6" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="V6" s="27" t="s">
+      <c r="D6" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="W6" s="22" t="s">
+      <c r="E6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AA6" s="26" t="s">
+      <c r="I6" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="AB6" s="25" t="s">
+      <c r="J6" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="K6" t="s">
         <v>91</v>
       </c>
-      <c r="AF6" s="26" t="s">
+      <c r="N6" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="19:32" x14ac:dyDescent="0.2">
-      <c r="S7" s="29">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="29">
         <v>9999999</v>
       </c>
-      <c r="T7" s="30" t="s">
+      <c r="B7" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="U7" s="22" t="s">
+      <c r="C7" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="V7" s="27" t="s">
+      <c r="D7" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="W7" s="22" t="s">
+      <c r="E7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="K7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="19:32" x14ac:dyDescent="0.2">
-      <c r="S8" s="28">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="28">
         <v>157710</v>
       </c>
-      <c r="T8" s="31" t="s">
+      <c r="B8" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="U8" s="22" t="s">
+      <c r="C8" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="V8" s="27" t="s">
+      <c r="D8" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="W8" s="22" t="s">
+      <c r="E8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AC8" s="28" t="s">
+      <c r="K8" s="28" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="19:32" x14ac:dyDescent="0.2">
-      <c r="S9" s="32">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="32">
         <v>66790</v>
       </c>
-      <c r="T9" s="33" t="s">
+      <c r="B9" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="U9" s="22" t="s">
+      <c r="C9" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="V9" s="27" t="s">
+      <c r="D9" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="W9" s="22" t="s">
+      <c r="E9" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AC9" s="32" t="s">
+      <c r="K9" s="32" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ISAICP-3443: Switch 'collection_logo', 'collection_banner', 'solution_logo', 'solution_banner' to 'file:*' migrations.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340"/>
   </bookViews>
   <sheets>
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="107">
   <si>
     <t>No</t>
   </si>
@@ -343,6 +343,18 @@
   </si>
   <si>
     <t>Community with 2 custom sections</t>
+  </si>
+  <si>
+    <t>acme.jpg</t>
+  </si>
+  <si>
+    <t>butterfly-wallpaper.jpg</t>
+  </si>
+  <si>
+    <t>Logo_1.png</t>
+  </si>
+  <si>
+    <t>Banner_1.png</t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1564,7 @@
   </sheetPr>
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1565,9 +1577,9 @@
     <col min="5" max="6" width="16.5" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" style="8" customWidth="1"/>
     <col min="12" max="12" width="9" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" style="8" customWidth="1"/>
@@ -2520,7 +2532,7 @@
       </c>
       <c r="S24" s="11"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="39" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>1</v>
       </c>
@@ -2543,8 +2555,12 @@
       <c r="H25" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
+      <c r="J25" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>104</v>
+      </c>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="14"/>
@@ -3041,8 +3057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="163" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="36.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3140,6 +3156,12 @@
       <c r="F3" s="23" t="s">
         <v>55</v>
       </c>
+      <c r="G3" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>106</v>
+      </c>
       <c r="I3" s="23" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
ISAICP-2920: Add a video in test cases.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -16,7 +16,7 @@
     <sheet name="5. Collections" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$38</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="108">
   <si>
     <t>No</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>Banner_1.png</t>
+  </si>
+  <si>
+    <t>Video</t>
   </si>
 </sst>
 </file>
@@ -548,7 +551,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="152">
+  <cellStyleXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -594,6 +597,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -801,7 +806,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="152">
+  <cellStyles count="154">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -930,6 +935,8 @@
     <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1266,8 +1273,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S37" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:S37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S38" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S38"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1562,7 +1569,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2532,7 +2539,7 @@
       </c>
       <c r="S24" s="11"/>
     </row>
-    <row r="25" spans="1:19" ht="39" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>1</v>
       </c>
@@ -3035,6 +3042,42 @@
       <c r="Q37" s="10"/>
       <c r="R37" s="10"/>
       <c r="S37" s="11"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="13">
+        <v>125838</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="34"/>
+      <c r="N38" s="34"/>
+      <c r="O38" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
ISAICP-3397: Add a new event test case with an invalid website URL.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -16,7 +16,7 @@
     <sheet name="5. Collections" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$39</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="109">
   <si>
     <t>No</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>Video</t>
+  </si>
+  <si>
+    <t>Event with invalid website URL</t>
   </si>
 </sst>
 </file>
@@ -551,7 +554,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="154">
+  <cellStyleXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -597,6 +600,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -806,7 +810,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="154">
+  <cellStyles count="155">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -937,6 +941,7 @@
     <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1273,8 +1278,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S38" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:S38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S39" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S39"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1569,7 +1574,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3078,6 +3083,42 @@
       <c r="Q38" s="10"/>
       <c r="R38" s="10"/>
       <c r="S38" s="11"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="13">
+        <v>42464</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
ISAICP-3478, ISAICP-3477: Collection OG user-roles (v2).
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -16,7 +16,7 @@
     <sheet name="5. Collections" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$40</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="112">
   <si>
     <t>No</t>
   </si>
@@ -361,13 +361,22 @@
   </si>
   <si>
     <t>Event with invalid website URL</t>
+  </si>
+  <si>
+    <t>Membership testing</t>
+  </si>
+  <si>
+    <t>lfalcon@gnusolidario.org</t>
+  </si>
+  <si>
+    <t>Project with various memberships</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,6 +439,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -469,55 +485,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right style="thin">
-        <color theme="4"/>
-      </right>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF5B9BD5"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF5B9BD5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF5B9BD5"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF5B9BD5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF5B9BD5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF5B9BD5"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF5B9BD5"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -534,27 +507,44 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF5B9BD5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF5B9BD5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5B9BD5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF5B9BD5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5B9BD5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="155">
+  <cellStyleXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -710,26 +700,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -740,38 +725,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -788,29 +749,42 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="155">
+  <cellStyles count="159">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -942,6 +916,10 @@
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1278,8 +1256,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S39" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:S39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S40" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S40"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1574,7 +1552,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1582,28 +1560,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.1640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.1640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="8" customWidth="1"/>
-    <col min="12" max="12" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" style="8" customWidth="1"/>
-    <col min="15" max="15" width="31.1640625" style="8" customWidth="1"/>
-    <col min="16" max="16" width="17.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="24.1640625" style="8"/>
+    <col min="1" max="1" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5" style="5" customWidth="1"/>
+    <col min="15" max="15" width="31.1640625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="24.1640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1613,1512 +1591,1587 @@
       <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="21" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="15">
         <v>60735</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="22" t="s">
+      <c r="H2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="11" t="s">
         <v>93</v>
       </c>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
     </row>
     <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="15">
         <v>99999999</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="22" t="s">
+      <c r="H3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="22"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="11"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="22" t="s">
+      <c r="G4" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="22"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10" t="s">
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="S4" s="11"/>
+      <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="15">
         <v>157729</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="22" t="s">
+      <c r="H5" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="22"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="11"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="15">
         <v>60736</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="8" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="11"/>
+      <c r="G6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="22"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="15">
         <v>58694</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="12" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="8" t="s">
+      <c r="G7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10" t="s">
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="11"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="15">
         <v>49860</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="12" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="8" t="s">
+      <c r="H8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10" t="s">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="M8" s="22" t="s">
         <v>75</v>
       </c>
       <c r="N8" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="15" t="s">
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="24" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="15">
         <v>87737</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="12" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="8" t="s">
+      <c r="G9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="22"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="10" t="s">
+      <c r="O9" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="11"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="15">
         <v>139528</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="12" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="8" t="s">
+      <c r="G10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10" t="s">
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="15" t="s">
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="24" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="15">
         <v>42233</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="12" t="s">
+      <c r="E11" s="7"/>
+      <c r="F11" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="8" t="s">
+      <c r="G11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10" t="s">
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="11"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="8"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="15">
         <v>138766</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="12" t="s">
+      <c r="E12" s="7"/>
+      <c r="F12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="8" t="s">
+      <c r="G12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10" t="s">
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="11"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="8"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="15">
         <v>133560</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="12" t="s">
+      <c r="E13" s="7"/>
+      <c r="F13" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="8" t="s">
+      <c r="G13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10" t="s">
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="11"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="8"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="15">
         <v>53012</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="12" t="s">
+      <c r="E14" s="7"/>
+      <c r="F14" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="8" t="s">
+      <c r="G14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10" t="s">
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="17"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="8"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="15">
         <v>63578</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="12" t="s">
+      <c r="E15" s="7"/>
+      <c r="F15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="8" t="s">
+      <c r="G15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10" t="s">
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="11"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="8"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="15">
         <v>155691</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="12" t="s">
+      <c r="E16" s="7"/>
+      <c r="F16" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="8" t="s">
+      <c r="G16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10" t="s">
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="11"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="8"/>
     </row>
     <row r="17" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="15">
         <v>27607</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="12" t="s">
+      <c r="E17" s="7"/>
+      <c r="F17" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="8" t="s">
+      <c r="G17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10" t="s">
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="15" t="s">
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="24" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="15">
         <v>155894</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="12" t="s">
+      <c r="E18" s="7"/>
+      <c r="F18" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="8" t="s">
+      <c r="G18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10" t="s">
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="11"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="8"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="15">
         <v>152066</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="12" t="s">
+      <c r="E19" s="7"/>
+      <c r="F19" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="8" t="s">
+      <c r="G19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10" t="s">
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="11"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="8"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="15">
         <v>145278</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="12" t="s">
+      <c r="E20" s="7"/>
+      <c r="F20" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="8" t="s">
+      <c r="G20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10" t="s">
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="11"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="8"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="15">
         <v>42438</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="18" t="s">
+      <c r="E21" s="7"/>
+      <c r="F21" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10" t="s">
+      <c r="H21" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="22"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M21" s="10" t="s">
+      <c r="M21" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="N21" s="10" t="s">
+      <c r="N21" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="O21" s="10" t="s">
+      <c r="O21" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="11"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="8"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="15">
         <v>149141</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="18" t="s">
+      <c r="E22" s="7"/>
+      <c r="F22" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H22" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10" t="s">
+      <c r="H22" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="22"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10" t="s">
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="11"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="15">
         <v>82307</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="18" t="s">
+      <c r="E23" s="7"/>
+      <c r="F23" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H23" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10" t="s">
+      <c r="H23" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="22"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10" t="s">
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10" t="s">
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S23" s="11"/>
+      <c r="S23" s="8"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="15">
         <v>76726</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="18" t="s">
+      <c r="E24" s="7"/>
+      <c r="F24" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H24" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10" t="s">
+      <c r="H24" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="22"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10" t="s">
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S24" s="11"/>
+      <c r="S24" s="8"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="15">
         <v>102713</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="18" t="s">
+      <c r="E25" s="7"/>
+      <c r="F25" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H25" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="10" t="s">
+      <c r="H25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="22"/>
+      <c r="J25" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="K25" s="10" t="s">
+      <c r="K25" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
       <c r="N25" s="14"/>
-      <c r="O25" s="10" t="s">
+      <c r="O25" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10" t="s">
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S25" s="11"/>
+      <c r="S25" s="8"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="15">
         <v>125548</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="18" t="s">
+      <c r="E26" s="7"/>
+      <c r="F26" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H26" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10" t="s">
+      <c r="H26" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="22"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10" t="s">
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S26" s="11"/>
+      <c r="S26" s="8"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="15">
         <v>42444</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="18" t="s">
+      <c r="E27" s="7"/>
+      <c r="F27" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H27" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10" t="s">
+      <c r="H27" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="22"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7" t="s">
         <v>76</v>
       </c>
       <c r="N27" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="O27" s="10" t="s">
+      <c r="O27" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10" t="s">
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S27" s="11"/>
+      <c r="S27" s="8"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="15">
         <v>150255</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="18" t="s">
+      <c r="E28" s="7"/>
+      <c r="F28" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H28" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10" t="s">
+      <c r="H28" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="22"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10" t="s">
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S28" s="11"/>
+      <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="15">
         <v>65803</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="18" t="s">
+      <c r="E29" s="7"/>
+      <c r="F29" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H29" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10" t="s">
+      <c r="H29" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="22"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10" t="s">
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S29" s="11"/>
+      <c r="S29" s="8"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="15">
         <v>156973</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="18" t="s">
+      <c r="E30" s="7"/>
+      <c r="F30" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G30" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H30" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10" t="s">
+      <c r="H30" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="22"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10" t="s">
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S30" s="11"/>
+      <c r="S30" s="8"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="15">
         <v>63567</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="18" t="s">
+      <c r="E31" s="7"/>
+      <c r="F31" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="8" t="s">
+      <c r="H31" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="22"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="22" t="s">
         <v>75</v>
       </c>
       <c r="N31" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="O31" s="10" t="s">
+      <c r="O31" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="10" t="s">
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S31" s="11"/>
+      <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="17">
         <v>59180</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="18" t="s">
+      <c r="E32" s="7"/>
+      <c r="F32" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H32" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10" t="s">
+      <c r="H32" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="22"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10" t="s">
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S32" s="11"/>
+      <c r="S32" s="8"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="17">
         <v>59183</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="18" t="s">
+      <c r="E33" s="7"/>
+      <c r="F33" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H33" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10" t="s">
+      <c r="H33" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="22"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10" t="s">
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S33" s="11"/>
+      <c r="S33" s="8"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="17">
         <v>60208</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="18" t="s">
+      <c r="E34" s="7"/>
+      <c r="F34" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10" t="s">
+      <c r="H34" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="22"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10" t="s">
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S34" s="11"/>
+      <c r="S34" s="8"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="13">
+      <c r="B35" s="17">
         <v>157710</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="18" t="s">
+      <c r="E35" s="7"/>
+      <c r="F35" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H35" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10" t="s">
+      <c r="H35" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="22"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M35" s="34"/>
-      <c r="N35" s="34"/>
-      <c r="O35" s="34" t="s">
+      <c r="M35" s="27"/>
+      <c r="N35" s="27"/>
+      <c r="O35" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="11"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="8"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="13">
+      <c r="B36" s="17">
         <v>27024</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="18" t="s">
+      <c r="E36" s="7"/>
+      <c r="F36" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H36" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="34" t="s">
+      <c r="H36" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="22"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="11"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="8"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="17">
         <v>66790</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="18" t="s">
+      <c r="E37" s="7"/>
+      <c r="F37" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G37" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H37" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10" t="s">
+      <c r="H37" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="22"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="34" t="s">
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="S37" s="11"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="8"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="13">
+      <c r="B38" s="17">
         <v>125838</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="18" t="s">
+      <c r="E38" s="7"/>
+      <c r="F38" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="G38" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H38" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
-      <c r="O38" s="34" t="s">
+      <c r="H38" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="22"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-      <c r="S38" s="11"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="13">
+      <c r="B39" s="17">
         <v>42464</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="18" t="s">
+      <c r="E39" s="7"/>
+      <c r="F39" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="G39" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H39" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34" t="s">
+      <c r="H39" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="22"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="11"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="8"/>
+    </row>
+    <row r="40" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="28">
+        <v>27026</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="22"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3139,10 +3192,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView zoomScale="163" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="36.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3164,232 +3217,284 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="31" t="s">
+    <row r="2" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="22" t="s">
+      <c r="E2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="23" t="s">
+    <row r="3" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="23" t="s">
+      <c r="E3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28">
+    <row r="4" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
         <v>42438</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26">
+    <row r="5" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="15">
         <v>149141</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28">
+    <row r="6" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
         <v>82307</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="N6" s="26" t="s">
+      <c r="N6" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="29">
+      <c r="A7" s="17">
         <v>9999999</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K7" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11" t="s">
         <v>92</v>
       </c>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="28">
+      <c r="A8" s="15">
         <v>157710</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K8" s="28" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="15" t="s">
         <v>97</v>
       </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="32">
+      <c r="A9" s="15">
         <v>66790</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="15" t="s">
         <v>101</v>
       </c>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>27026</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ISAICP-3429: Migrate solution and release documentation with unlimited cardinality.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -16,7 +16,7 @@
     <sheet name="5. Collections" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$41</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="113">
   <si>
     <t>No</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>Project with various memberships</t>
+  </si>
+  <si>
+    <t>Project with multipe documentation files</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -704,8 +707,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -783,8 +787,20 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="160">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -920,6 +936,7 @@
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1256,8 +1273,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S40" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:S40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S41" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S41"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1552,7 +1569,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3172,6 +3189,42 @@
       <c r="Q40" s="7"/>
       <c r="R40" s="7"/>
       <c r="S40" s="8"/>
+    </row>
+    <row r="41" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="30">
+        <v>68304</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" s="29"/>
+      <c r="F41" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="P41" s="29"/>
+      <c r="Q41" s="29"/>
+      <c r="R41" s="29"/>
+      <c r="S41" s="32"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
ISAICP-3496: Switch to the version v1.20 of the content mapping Excel file.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -16,7 +16,7 @@
     <sheet name="5. Collections" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$S$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$T$41</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="115">
   <si>
     <t>No</t>
   </si>
@@ -373,13 +373,19 @@
   </si>
   <si>
     <t>Project with multipe documentation files</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Description for a new collection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,8 +455,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,8 +501,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -546,6 +566,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF5B9BD5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF5B9BD5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5B9BD5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -709,7 +768,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -740,9 +799,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -797,6 +853,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -962,7 +1025,32 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1273,31 +1361,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:S41" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:S41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:T41" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:T41"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
-  <tableColumns count="19">
-    <tableColumn id="20" name="Type of content item" dataDxfId="18"/>
-    <tableColumn id="18" name="Nid" dataDxfId="17" dataCellStyle="Normale 2"/>
-    <tableColumn id="1" name="Title of content item" dataDxfId="16"/>
-    <tableColumn id="10" name="Collection_Name" dataDxfId="15"/>
-    <tableColumn id="3" name="Policy domain 1" dataDxfId="14"/>
-    <tableColumn id="27" name="Policy domain 2" dataDxfId="13" dataCellStyle="Normale 2"/>
-    <tableColumn id="22" name="New collection" dataDxfId="12"/>
-    <tableColumn id="30" name="Migrate" dataDxfId="11" dataCellStyle="Normale 2"/>
-    <tableColumn id="12" name="Abstract" dataDxfId="10"/>
-    <tableColumn id="8" name="Logo" dataDxfId="9"/>
-    <tableColumn id="2" name="Banner" dataDxfId="8"/>
-    <tableColumn id="15" name="Owner" dataDxfId="7"/>
-    <tableColumn id="5" name="Owner name" dataDxfId="6" dataCellStyle="Normale 2"/>
-    <tableColumn id="4" name="Owner type" dataDxfId="5" dataCellStyle="Normale 2"/>
-    <tableColumn id="9" name="Collection Owner" dataDxfId="4" dataCellStyle="Normale 2"/>
-    <tableColumn id="25" name="Elibrary Creation" dataDxfId="3"/>
-    <tableColumn id="26" name="Pre Moderation" dataDxfId="2"/>
-    <tableColumn id="13" name="Collection state" dataDxfId="1"/>
-    <tableColumn id="28" name="Content item state" dataDxfId="0" dataCellStyle="Normale 2"/>
+  <tableColumns count="20">
+    <tableColumn id="20" name="Type of content item" dataDxfId="19"/>
+    <tableColumn id="18" name="Nid" dataDxfId="18" dataCellStyle="Normale 2"/>
+    <tableColumn id="1" name="Title of content item" dataDxfId="17"/>
+    <tableColumn id="10" name="Collection_Name" dataDxfId="16"/>
+    <tableColumn id="3" name="Policy domain 1" dataDxfId="15"/>
+    <tableColumn id="27" name="Policy domain 2" dataDxfId="14" dataCellStyle="Normale 2"/>
+    <tableColumn id="22" name="New collection" dataDxfId="13"/>
+    <tableColumn id="30" name="Migrate" dataDxfId="12" dataCellStyle="Normale 2"/>
+    <tableColumn id="6" name="Description" dataDxfId="0" dataCellStyle="Normale 2"/>
+    <tableColumn id="12" name="Abstract" dataDxfId="11"/>
+    <tableColumn id="8" name="Logo" dataDxfId="10"/>
+    <tableColumn id="2" name="Banner" dataDxfId="9"/>
+    <tableColumn id="15" name="Owner" dataDxfId="8"/>
+    <tableColumn id="5" name="Owner name" dataDxfId="7" dataCellStyle="Normale 2"/>
+    <tableColumn id="4" name="Owner type" dataDxfId="6" dataCellStyle="Normale 2"/>
+    <tableColumn id="9" name="Collection Owner" dataDxfId="5" dataCellStyle="Normale 2"/>
+    <tableColumn id="25" name="Elibrary Creation" dataDxfId="4"/>
+    <tableColumn id="26" name="Pre Moderation" dataDxfId="3"/>
+    <tableColumn id="13" name="Collection state" dataDxfId="2"/>
+    <tableColumn id="28" name="Content item state" dataDxfId="1" dataCellStyle="Normale 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1569,7 +1658,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1584,21 +1673,22 @@
     <col min="5" max="6" width="16.5" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" style="5" customWidth="1"/>
-    <col min="15" max="15" width="31.1640625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="17.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="24.1640625" style="5"/>
+    <col min="9" max="9" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5" style="5" customWidth="1"/>
+    <col min="16" max="16" width="31.1640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="17.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="24.1640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1623,213 +1713,220 @@
       <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="N1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="O1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="P1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="S1" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="T1" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>60735</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="11" t="s">
+      <c r="H2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-    </row>
-    <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+    </row>
+    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>99999999</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>95</v>
       </c>
       <c r="E3" s="7"/>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="7"/>
+      <c r="H3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="7"/>
+      <c r="P3" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
-      <c r="S3" s="8"/>
-    </row>
-    <row r="4" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S3" s="7"/>
+      <c r="T3" s="8"/>
+    </row>
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>95</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="22"/>
-      <c r="J4" s="7"/>
+      <c r="G4" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="7"/>
+      <c r="P4" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="7"/>
+      <c r="S4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="S4" s="8"/>
-    </row>
-    <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="T4" s="8"/>
+    </row>
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>157729</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>95</v>
       </c>
       <c r="E5" s="7"/>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="7"/>
+      <c r="H5" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="7"/>
+      <c r="P5" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
-      <c r="S5" s="8"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S5" s="7"/>
+      <c r="T5" s="8"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>60736</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="7"/>
+      <c r="G6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -1838,653 +1935,672 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
-      <c r="S6" s="8"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S6" s="7"/>
+      <c r="T6" s="8"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>58694</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="22" t="s">
+      <c r="H7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="7"/>
+      <c r="P7" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
-      <c r="S7" s="8"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S7" s="7"/>
+      <c r="T7" s="8"/>
+    </row>
+    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>49860</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="22" t="s">
+      <c r="H8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="J8" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="7"/>
+      <c r="M8" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M8" s="22" t="s">
+      <c r="N8" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="O8" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="P8" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
-      <c r="S8" s="24" t="s">
+      <c r="S8" s="7"/>
+      <c r="T8" s="23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>87737</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="22" t="s">
+      <c r="H9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="7" t="s">
+      <c r="M9" s="7"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
-      <c r="S9" s="8"/>
-    </row>
-    <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S9" s="7"/>
+      <c r="T9" s="8"/>
+    </row>
+    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>139528</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="22" t="s">
+      <c r="H10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
-      <c r="O10" s="7" t="s">
+      <c r="O10" s="7"/>
+      <c r="P10" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
-      <c r="S10" s="24" t="s">
+      <c r="S10" s="7"/>
+      <c r="T10" s="23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>42233</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="22" t="s">
+      <c r="H11" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
-      <c r="O11" s="7" t="s">
+      <c r="O11" s="7"/>
+      <c r="P11" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
-      <c r="S11" s="8"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S11" s="7"/>
+      <c r="T11" s="8"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>138766</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="22" t="s">
+      <c r="H12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="7" t="s">
+      <c r="O12" s="7"/>
+      <c r="P12" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
-      <c r="S12" s="8"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S12" s="7"/>
+      <c r="T12" s="8"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>133560</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="22" t="s">
+      <c r="H13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
-      <c r="O13" s="7" t="s">
+      <c r="O13" s="7"/>
+      <c r="P13" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
-      <c r="S13" s="8"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S13" s="7"/>
+      <c r="T13" s="8"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>53012</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="22" t="s">
+      <c r="H14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="7" t="s">
+      <c r="O14" s="7"/>
+      <c r="P14" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
-      <c r="S14" s="8"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S14" s="7"/>
+      <c r="T14" s="8"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>63578</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="22" t="s">
+      <c r="H15" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
-      <c r="O15" s="7" t="s">
+      <c r="O15" s="7"/>
+      <c r="P15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
-      <c r="S15" s="8"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S15" s="7"/>
+      <c r="T15" s="8"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>155691</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="22" t="s">
+      <c r="H16" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
-      <c r="O16" s="7" t="s">
+      <c r="O16" s="7"/>
+      <c r="P16" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
-      <c r="S16" s="8"/>
-    </row>
-    <row r="17" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S16" s="7"/>
+      <c r="T16" s="8"/>
+    </row>
+    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>27607</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="22" t="s">
+      <c r="H17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
-      <c r="O17" s="7" t="s">
+      <c r="O17" s="7"/>
+      <c r="P17" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
-      <c r="S17" s="24" t="s">
+      <c r="S17" s="7"/>
+      <c r="T17" s="23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>155894</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="22" t="s">
+      <c r="H18" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
-      <c r="O18" s="7" t="s">
+      <c r="O18" s="7"/>
+      <c r="P18" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
-      <c r="S18" s="8"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S18" s="7"/>
+      <c r="T18" s="8"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <v>152066</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="7"/>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="22" t="s">
+      <c r="H19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="16"/>
+      <c r="J19" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
-      <c r="O19" s="7" t="s">
+      <c r="O19" s="7"/>
+      <c r="P19" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
-      <c r="S19" s="8"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S19" s="7"/>
+      <c r="T19" s="8"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="14">
         <v>145278</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="22" t="s">
+      <c r="H20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="16"/>
+      <c r="J20" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
-      <c r="O20" s="7" t="s">
+      <c r="O20" s="7"/>
+      <c r="P20" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
-      <c r="S20" s="8"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S20" s="7"/>
+      <c r="T20" s="8"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>42438</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="21" t="s">
         <v>88</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H21" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="22"/>
-      <c r="J21" s="7"/>
+      <c r="H21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="16"/>
+      <c r="J21" s="21"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="7" t="s">
+      <c r="L21" s="7"/>
+      <c r="M21" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M21" s="7" t="s">
+      <c r="N21" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="N21" s="7" t="s">
+      <c r="O21" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="O21" s="7" t="s">
+      <c r="P21" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
-      <c r="S21" s="8"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S21" s="7"/>
+      <c r="T21" s="8"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="14">
         <v>149141</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="21" t="s">
         <v>53</v>
       </c>
       <c r="E22" s="7"/>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="25" t="s">
         <v>54</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H22" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="22"/>
-      <c r="J22" s="7"/>
+      <c r="H22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="16"/>
+      <c r="J22" s="21"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="7" t="s">
+      <c r="L22" s="7"/>
+      <c r="M22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M22" s="7"/>
       <c r="N22" s="7"/>
-      <c r="O22" s="7" t="s">
+      <c r="O22" s="7"/>
+      <c r="P22" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
-      <c r="S22" s="8"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S22" s="7"/>
+      <c r="T22" s="8"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="14">
         <v>82307</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -2494,38 +2610,39 @@
         <v>59</v>
       </c>
       <c r="E23" s="7"/>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H23" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="22"/>
-      <c r="J23" s="7"/>
+      <c r="H23" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="16"/>
+      <c r="J23" s="21"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="7" t="s">
+      <c r="L23" s="7"/>
+      <c r="M23" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M23" s="7"/>
       <c r="N23" s="7"/>
-      <c r="O23" s="7" t="s">
+      <c r="O23" s="7"/>
+      <c r="P23" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
-      <c r="R23" s="7" t="s">
+      <c r="R23" s="7"/>
+      <c r="S23" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S23" s="8"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T23" s="8"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="14">
         <v>76726</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -2535,36 +2652,37 @@
         <v>59</v>
       </c>
       <c r="E24" s="7"/>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H24" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="22"/>
-      <c r="J24" s="7"/>
+      <c r="H24" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="16"/>
+      <c r="J24" s="21"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
-      <c r="O24" s="7" t="s">
+      <c r="O24" s="7"/>
+      <c r="P24" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
-      <c r="R24" s="7" t="s">
+      <c r="R24" s="7"/>
+      <c r="S24" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S24" s="8"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T24" s="8"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="14">
         <v>102713</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -2574,40 +2692,41 @@
         <v>59</v>
       </c>
       <c r="E25" s="7"/>
-      <c r="F25" s="26" t="s">
+      <c r="F25" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H25" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="22"/>
-      <c r="J25" s="7" t="s">
+      <c r="H25" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="16"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="L25" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="L25" s="7"/>
       <c r="M25" s="7"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="7" t="s">
+      <c r="N25" s="7"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
-      <c r="R25" s="7" t="s">
+      <c r="R25" s="7"/>
+      <c r="S25" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S25" s="8"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T25" s="8"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="14">
         <v>125548</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -2617,36 +2736,37 @@
         <v>59</v>
       </c>
       <c r="E26" s="7"/>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H26" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="22"/>
-      <c r="J26" s="7"/>
+      <c r="H26" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="16"/>
+      <c r="J26" s="21"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
-      <c r="O26" s="7" t="s">
+      <c r="O26" s="7"/>
+      <c r="P26" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
-      <c r="R26" s="7" t="s">
+      <c r="R26" s="7"/>
+      <c r="S26" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S26" s="8"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T26" s="8"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="14">
         <v>42444</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -2656,40 +2776,41 @@
         <v>59</v>
       </c>
       <c r="E27" s="7"/>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H27" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="22"/>
-      <c r="J27" s="7"/>
+      <c r="H27" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="16"/>
+      <c r="J27" s="21"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
-      <c r="M27" s="7" t="s">
+      <c r="M27" s="7"/>
+      <c r="N27" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="N27" s="14" t="s">
+      <c r="O27" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="O27" s="7" t="s">
+      <c r="P27" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
-      <c r="R27" s="7" t="s">
+      <c r="R27" s="7"/>
+      <c r="S27" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S27" s="8"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T27" s="8"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <v>150255</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -2699,36 +2820,37 @@
         <v>59</v>
       </c>
       <c r="E28" s="7"/>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H28" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="22"/>
-      <c r="J28" s="7"/>
+      <c r="H28" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="16"/>
+      <c r="J28" s="21"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="7" t="s">
+      <c r="O28" s="7"/>
+      <c r="P28" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
-      <c r="R28" s="7" t="s">
+      <c r="R28" s="7"/>
+      <c r="S28" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S28" s="8"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T28" s="8"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="14">
         <v>65803</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -2738,36 +2860,37 @@
         <v>59</v>
       </c>
       <c r="E29" s="7"/>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H29" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="22"/>
-      <c r="J29" s="7"/>
+      <c r="H29" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="16"/>
+      <c r="J29" s="21"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
-      <c r="O29" s="7" t="s">
+      <c r="O29" s="7"/>
+      <c r="P29" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
-      <c r="R29" s="7" t="s">
+      <c r="R29" s="7"/>
+      <c r="S29" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S29" s="8"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T29" s="8"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="14">
         <v>156973</v>
       </c>
       <c r="C30" s="7" t="s">
@@ -2777,36 +2900,37 @@
         <v>59</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H30" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="22"/>
-      <c r="J30" s="7"/>
+      <c r="H30" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="16"/>
+      <c r="J30" s="21"/>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
-      <c r="O30" s="7" t="s">
+      <c r="O30" s="7"/>
+      <c r="P30" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
-      <c r="R30" s="7" t="s">
+      <c r="R30" s="7"/>
+      <c r="S30" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S30" s="8"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T30" s="8"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="14">
         <v>63567</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -2816,40 +2940,41 @@
         <v>59</v>
       </c>
       <c r="E31" s="7"/>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H31" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="22"/>
-      <c r="J31" s="7"/>
+      <c r="H31" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="16"/>
+      <c r="J31" s="21"/>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
-      <c r="M31" s="22" t="s">
+      <c r="M31" s="7"/>
+      <c r="N31" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="N31" s="14" t="s">
+      <c r="O31" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="O31" s="7" t="s">
+      <c r="P31" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
-      <c r="R31" s="7" t="s">
+      <c r="R31" s="7"/>
+      <c r="S31" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S31" s="8"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T31" s="8"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="17">
+      <c r="B32" s="16">
         <v>59180</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -2859,36 +2984,37 @@
         <v>59</v>
       </c>
       <c r="E32" s="7"/>
-      <c r="F32" s="26" t="s">
+      <c r="F32" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H32" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="22"/>
-      <c r="J32" s="7"/>
+      <c r="H32" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="16"/>
+      <c r="J32" s="21"/>
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
-      <c r="O32" s="7" t="s">
+      <c r="O32" s="7"/>
+      <c r="P32" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
-      <c r="R32" s="7" t="s">
+      <c r="R32" s="7"/>
+      <c r="S32" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S32" s="8"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T32" s="8"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="17">
+      <c r="B33" s="16">
         <v>59183</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -2898,36 +3024,37 @@
         <v>59</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="26" t="s">
+      <c r="F33" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H33" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="22"/>
-      <c r="J33" s="7"/>
+      <c r="H33" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="16"/>
+      <c r="J33" s="21"/>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
-      <c r="O33" s="7" t="s">
+      <c r="O33" s="7"/>
+      <c r="P33" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
-      <c r="R33" s="7" t="s">
+      <c r="R33" s="7"/>
+      <c r="S33" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S33" s="8"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T33" s="8"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B34" s="16">
         <v>60208</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -2937,303 +3064,311 @@
         <v>59</v>
       </c>
       <c r="E34" s="7"/>
-      <c r="F34" s="26" t="s">
+      <c r="F34" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H34" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" s="22"/>
-      <c r="J34" s="7"/>
+      <c r="H34" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="16"/>
+      <c r="J34" s="21"/>
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
-      <c r="O34" s="7" t="s">
+      <c r="O34" s="7"/>
+      <c r="P34" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
-      <c r="R34" s="7" t="s">
+      <c r="R34" s="7"/>
+      <c r="S34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S34" s="8"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T34" s="8"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="17">
+      <c r="B35" s="16">
         <v>157710</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="21" t="s">
         <v>98</v>
       </c>
       <c r="E35" s="7"/>
-      <c r="F35" s="26" t="s">
+      <c r="F35" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H35" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="22"/>
-      <c r="J35" s="7"/>
+      <c r="H35" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="16"/>
+      <c r="J35" s="21"/>
       <c r="K35" s="7"/>
-      <c r="L35" s="7" t="s">
+      <c r="L35" s="7"/>
+      <c r="M35" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="27" t="s">
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="7"/>
-      <c r="S35" s="8"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S35" s="7"/>
+      <c r="T35" s="8"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="17">
+      <c r="B36" s="16">
         <v>27024</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="21" t="s">
         <v>98</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="26" t="s">
+      <c r="F36" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H36" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="22"/>
-      <c r="J36" s="7"/>
+      <c r="H36" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="16"/>
+      <c r="J36" s="21"/>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="27" t="s">
+      <c r="M36" s="7"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="P36" s="7"/>
       <c r="Q36" s="7"/>
       <c r="R36" s="7"/>
-      <c r="S36" s="8"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S36" s="7"/>
+      <c r="T36" s="8"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B37" s="16">
         <v>66790</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="21" t="s">
         <v>100</v>
       </c>
       <c r="E37" s="7"/>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G37" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H37" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="22"/>
-      <c r="J37" s="7"/>
+      <c r="H37" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="16"/>
+      <c r="J37" s="21"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="7" t="s">
+      <c r="L37" s="7"/>
+      <c r="M37" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
-      <c r="O37" s="27" t="s">
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="7"/>
-      <c r="S37" s="8"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S37" s="7"/>
+      <c r="T37" s="8"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="17">
+      <c r="B38" s="16">
         <v>125838</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="21" t="s">
         <v>100</v>
       </c>
       <c r="E38" s="7"/>
-      <c r="F38" s="26" t="s">
+      <c r="F38" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H38" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="22"/>
-      <c r="J38" s="7"/>
+      <c r="H38" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="16"/>
+      <c r="J38" s="21"/>
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="27" t="s">
+      <c r="M38" s="7"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="P38" s="7"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="7"/>
-      <c r="S38" s="8"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S38" s="7"/>
+      <c r="T38" s="8"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="16">
         <v>42464</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="21" t="s">
         <v>100</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="26" t="s">
+      <c r="F39" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H39" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="22"/>
-      <c r="J39" s="7"/>
+      <c r="H39" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="16"/>
+      <c r="J39" s="21"/>
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="27" t="s">
+      <c r="M39" s="7"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
+      <c r="P39" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7"/>
-      <c r="S39" s="8"/>
-    </row>
-    <row r="40" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="S39" s="7"/>
+      <c r="T39" s="8"/>
+    </row>
+    <row r="40" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="28">
+      <c r="B40" s="27">
         <v>27026</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D40" s="17" t="s">
         <v>109</v>
       </c>
       <c r="E40" s="7"/>
-      <c r="F40" s="26" t="s">
+      <c r="F40" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H40" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="22"/>
-      <c r="J40" s="7"/>
+      <c r="H40" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="16"/>
+      <c r="J40" s="21"/>
       <c r="K40" s="7"/>
-      <c r="L40" s="7" t="s">
+      <c r="L40" s="7"/>
+      <c r="M40" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="11" t="s">
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
       <c r="R40" s="7"/>
-      <c r="S40" s="8"/>
-    </row>
-    <row r="41" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="s">
+      <c r="S40" s="7"/>
+      <c r="T40" s="8"/>
+    </row>
+    <row r="41" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="30">
+      <c r="B41" s="29">
         <v>68304</v>
       </c>
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E41" s="29"/>
-      <c r="F41" s="26" t="s">
+      <c r="E41" s="28"/>
+      <c r="F41" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H41" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J41" s="29"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="11" t="s">
+      <c r="H41" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="16"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="28"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="P41" s="29"/>
-      <c r="Q41" s="29"/>
-      <c r="R41" s="29"/>
-      <c r="S41" s="32"/>
+      <c r="Q41" s="28"/>
+      <c r="R41" s="28"/>
+      <c r="S41" s="28"/>
+      <c r="T41" s="31"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O7" r:id="rId1" display="doe@example.com"/>
-    <hyperlink ref="O21" r:id="rId2" display="baby.doe@example.com"/>
-    <hyperlink ref="O23" r:id="rId3" display="doe@example.com"/>
-    <hyperlink ref="O8:O19" r:id="rId4" display="doe@example.com"/>
-    <hyperlink ref="O20" r:id="rId5" display="doe@example.com"/>
-    <hyperlink ref="O24:O34" r:id="rId6" display="doe@example.com"/>
+    <hyperlink ref="P7" r:id="rId1" display="doe@example.com"/>
+    <hyperlink ref="P21" r:id="rId2" display="baby.doe@example.com"/>
+    <hyperlink ref="P23" r:id="rId3" display="doe@example.com"/>
+    <hyperlink ref="P8:P19" r:id="rId4" display="doe@example.com"/>
+    <hyperlink ref="P20" r:id="rId5" display="doe@example.com"/>
+    <hyperlink ref="P24:P34" r:id="rId6" display="doe@example.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -3245,7 +3380,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView zoomScale="163" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3258,18 +3393,19 @@
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>66</v>
       </c>
@@ -3285,35 +3421,38 @@
       <c r="E1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>95</v>
       </c>
@@ -3326,44 +3465,47 @@
       <c r="E2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="E3" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15">
+    <row r="4" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
         <v>42438</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -3372,24 +3514,24 @@
       <c r="C4" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="K4" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15">
+    <row r="5" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
         <v>149141</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -3398,56 +3540,56 @@
       <c r="C5" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>54</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="L5" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15">
+    <row r="6" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
         <v>82307</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="J6" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="K6" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="N6" s="15" t="s">
+      <c r="O6" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="17">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="16">
         <v>9999999</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>86</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -3458,15 +3600,16 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="11"/>
+      <c r="L7" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="L7" s="11"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="15">
+      <c r="O7" s="11"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
         <v>157710</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -3475,7 +3618,7 @@
       <c r="C8" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -3486,15 +3629,16 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="11"/>
+      <c r="L8" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="L8" s="11"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
+      <c r="O8" s="11"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
         <v>66790</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -3503,7 +3647,7 @@
       <c r="C9" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -3514,24 +3658,25 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="11"/>
+      <c r="L9" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="11"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>27026</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>109</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E10" s="11" t="s">
@@ -3542,12 +3687,13 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="11"/>
+      <c r="L10" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="L10" s="11"/>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ISAICP-3502: New URL column in Excel file, tab "5. Collections".
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="117">
   <si>
     <t>No</t>
   </si>
@@ -379,6 +379,12 @@
   </si>
   <si>
     <t>Description for a new collection</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>http://example.com/this_collection</t>
   </si>
 </sst>
 </file>
@@ -606,7 +612,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="160">
+  <cellStyleXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -767,8 +773,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -862,8 +869,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="160">
+  <cellStyles count="161">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1000,6 +1008,7 @@
     <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1026,31 +1035,6 @@
     <cellStyle name="Normale 2" xfId="1"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1266,6 +1250,31 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1375,18 +1384,18 @@
     <tableColumn id="27" name="Policy domain 2" dataDxfId="14" dataCellStyle="Normale 2"/>
     <tableColumn id="22" name="New collection" dataDxfId="13"/>
     <tableColumn id="30" name="Migrate" dataDxfId="12" dataCellStyle="Normale 2"/>
-    <tableColumn id="6" name="Description" dataDxfId="0" dataCellStyle="Normale 2"/>
-    <tableColumn id="12" name="Abstract" dataDxfId="11"/>
-    <tableColumn id="8" name="Logo" dataDxfId="10"/>
-    <tableColumn id="2" name="Banner" dataDxfId="9"/>
-    <tableColumn id="15" name="Owner" dataDxfId="8"/>
-    <tableColumn id="5" name="Owner name" dataDxfId="7" dataCellStyle="Normale 2"/>
-    <tableColumn id="4" name="Owner type" dataDxfId="6" dataCellStyle="Normale 2"/>
-    <tableColumn id="9" name="Collection Owner" dataDxfId="5" dataCellStyle="Normale 2"/>
-    <tableColumn id="25" name="Elibrary Creation" dataDxfId="4"/>
-    <tableColumn id="26" name="Pre Moderation" dataDxfId="3"/>
-    <tableColumn id="13" name="Collection state" dataDxfId="2"/>
-    <tableColumn id="28" name="Content item state" dataDxfId="1" dataCellStyle="Normale 2"/>
+    <tableColumn id="6" name="Description" dataDxfId="11" dataCellStyle="Normale 2"/>
+    <tableColumn id="12" name="Abstract" dataDxfId="10"/>
+    <tableColumn id="8" name="Logo" dataDxfId="9"/>
+    <tableColumn id="2" name="Banner" dataDxfId="8"/>
+    <tableColumn id="15" name="Owner" dataDxfId="7"/>
+    <tableColumn id="5" name="Owner name" dataDxfId="6" dataCellStyle="Normale 2"/>
+    <tableColumn id="4" name="Owner type" dataDxfId="5" dataCellStyle="Normale 2"/>
+    <tableColumn id="9" name="Collection Owner" dataDxfId="4" dataCellStyle="Normale 2"/>
+    <tableColumn id="25" name="Elibrary Creation" dataDxfId="3"/>
+    <tableColumn id="26" name="Pre Moderation" dataDxfId="2"/>
+    <tableColumn id="13" name="Collection state" dataDxfId="1"/>
+    <tableColumn id="28" name="Content item state" dataDxfId="0" dataCellStyle="Normale 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3380,7 +3389,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScale="163" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3403,9 +3412,10 @@
     <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>66</v>
       </c>
@@ -3451,8 +3461,11 @@
       <c r="O1" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P1" s="35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>95</v>
       </c>
@@ -3469,7 +3482,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>9</v>
       </c>
@@ -3504,7 +3517,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>42438</v>
       </c>
@@ -3530,7 +3543,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
         <v>149141</v>
       </c>
@@ -3549,8 +3562,11 @@
       <c r="L5" s="11" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P5" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>82307</v>
       </c>
@@ -3579,7 +3595,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
         <v>9999999</v>
       </c>
@@ -3608,7 +3624,7 @@
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
         <v>157710</v>
       </c>
@@ -3637,7 +3653,7 @@
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
         <v>66790</v>
       </c>
@@ -3666,7 +3682,7 @@
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>27026</v>
       </c>

</xml_diff>

<commit_message>
Add 'The Re3gistry' as testing case to check solution OG membership.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
     <sheet name="5. Collections" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$T$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$T$42</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="118">
   <si>
     <t>No</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>http://example.com/this_collection</t>
+  </si>
+  <si>
+    <t>Member test</t>
   </si>
 </sst>
 </file>
@@ -1370,8 +1373,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:T41" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:T41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:T42" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:T42"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1667,9 +1670,9 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:T41"/>
+  <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3370,6 +3373,43 @@
       <c r="S41" s="28"/>
       <c r="T41" s="31"/>
     </row>
+    <row r="42" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="29">
+        <v>68202</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="16"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="30"/>
+      <c r="O42" s="30"/>
+      <c r="P42" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="31"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="P7" r:id="rId1" display="doe@example.com"/>
@@ -3391,7 +3431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView zoomScale="163" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Revert "Add 'The Re3gistry' as testing case to check solution OG membership."
This reverts commit 887a4aec39b03611ca27f7e2a5ea3bd0df4beac7.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340"/>
   </bookViews>
   <sheets>
     <sheet name="1. Content items" sheetId="2" r:id="rId1"/>
     <sheet name="5. Collections" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$T$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$T$41</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="117">
   <si>
     <t>No</t>
   </si>
@@ -385,9 +385,6 @@
   </si>
   <si>
     <t>http://example.com/this_collection</t>
-  </si>
-  <si>
-    <t>Member test</t>
   </si>
 </sst>
 </file>
@@ -1373,8 +1370,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:T42" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:T42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:T41" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:T41"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1670,9 +1667,9 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3373,43 +3370,6 @@
       <c r="S41" s="28"/>
       <c r="T41" s="31"/>
     </row>
-    <row r="42" spans="1:20" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" s="29">
-        <v>68202</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E42" s="28"/>
-      <c r="F42" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="16"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="30"/>
-      <c r="O42" s="30"/>
-      <c r="P42" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q42" s="28"/>
-      <c r="R42" s="28"/>
-      <c r="S42" s="28"/>
-      <c r="T42" s="31"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="P7" r:id="rId1" display="doe@example.com"/>
@@ -3431,7 +3391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+    <sheetView zoomScale="163" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ISAICP-3672: Tests are running again. Tidied up the test DB from 270 to 6MB.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -303,24 +303,6 @@
     <t>Collection from Project</t>
   </si>
   <si>
-    <t>joel@sambreville.be</t>
-  </si>
-  <si>
-    <t>viktor.hristov@hotmail.com</t>
-  </si>
-  <si>
-    <t>eric.smets@fks.be</t>
-  </si>
-  <si>
-    <t>mux2005@gmail.com</t>
-  </si>
-  <si>
-    <t>riccardo.sibilia@vtg.admin.ch</t>
-  </si>
-  <si>
-    <t>tbenita@atreal.fr, aanguix@gvsig.com</t>
-  </si>
-  <si>
     <t>Collection with erroneous items</t>
   </si>
   <si>
@@ -366,9 +348,6 @@
     <t>Membership testing</t>
   </si>
   <si>
-    <t>lfalcon@gnusolidario.org</t>
-  </si>
-  <si>
     <t>Project with various memberships</t>
   </si>
   <si>
@@ -385,6 +364,27 @@
   </si>
   <si>
     <t>http://example.com/this_collection</t>
+  </si>
+  <si>
+    <t>user7143@example.com</t>
+  </si>
+  <si>
+    <t>user7098@example.com</t>
+  </si>
+  <si>
+    <t>user7160@example.com</t>
+  </si>
+  <si>
+    <t>user7051@example.com</t>
+  </si>
+  <si>
+    <t>user7287@example.com, user6416@example.com</t>
+  </si>
+  <si>
+    <t>user7021@example.com</t>
+  </si>
+  <si>
+    <t>user9351@example.com</t>
   </si>
 </sst>
 </file>
@@ -1723,7 +1723,7 @@
         <v>15</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
@@ -1790,7 +1790,7 @@
       <c r="N2" s="21"/>
       <c r="O2" s="21"/>
       <c r="P2" s="11" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="Q2" s="21"/>
       <c r="R2" s="21"/>
@@ -1808,7 +1808,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="21" t="s">
@@ -1828,7 +1828,7 @@
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
       <c r="P3" s="11" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
@@ -1846,7 +1846,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="21" t="s">
@@ -1866,7 +1866,7 @@
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="11" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
@@ -1886,7 +1886,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="21" t="s">
@@ -1906,7 +1906,7 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="11" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
@@ -1980,7 +1980,7 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
@@ -2011,7 +2011,7 @@
         <v>16</v>
       </c>
       <c r="I8" s="34" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="J8" s="21" t="s">
         <v>55</v>
@@ -2028,7 +2028,7 @@
         <v>73</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
@@ -2070,7 +2070,7 @@
       <c r="N9" s="21"/>
       <c r="O9" s="13"/>
       <c r="P9" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
@@ -2110,7 +2110,7 @@
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
@@ -2152,7 +2152,7 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
@@ -2192,7 +2192,7 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
@@ -2232,7 +2232,7 @@
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
@@ -2272,7 +2272,7 @@
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
@@ -2312,7 +2312,7 @@
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
@@ -2352,7 +2352,7 @@
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
@@ -2392,7 +2392,7 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
@@ -2434,7 +2434,7 @@
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
@@ -2474,7 +2474,7 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
@@ -2514,7 +2514,7 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
@@ -2558,14 +2558,14 @@
         <v>73</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
       <c r="T21" s="8"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
@@ -2597,8 +2597,8 @@
       </c>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
-      <c r="P22" s="7" t="s">
-        <v>94</v>
+      <c r="P22" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
@@ -2638,7 +2638,7 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
@@ -2678,7 +2678,7 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
@@ -2713,16 +2713,16 @@
       <c r="I25" s="16"/>
       <c r="J25" s="21"/>
       <c r="K25" s="7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
       <c r="O25" s="13"/>
       <c r="P25" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
@@ -2762,7 +2762,7 @@
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q26" s="7"/>
       <c r="R26" s="7"/>
@@ -2806,7 +2806,7 @@
         <v>74</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
@@ -2846,7 +2846,7 @@
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
       <c r="P28" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
@@ -2886,7 +2886,7 @@
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q29" s="7"/>
       <c r="R29" s="7"/>
@@ -2926,7 +2926,7 @@
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
       <c r="P30" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q30" s="7"/>
       <c r="R30" s="7"/>
@@ -2970,7 +2970,7 @@
         <v>73</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q31" s="7"/>
       <c r="R31" s="7"/>
@@ -3010,7 +3010,7 @@
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
       <c r="P32" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q32" s="7"/>
       <c r="R32" s="7"/>
@@ -3050,7 +3050,7 @@
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
       <c r="P33" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q33" s="7"/>
       <c r="R33" s="7"/>
@@ -3090,7 +3090,7 @@
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
       <c r="P34" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="Q34" s="7"/>
       <c r="R34" s="7"/>
@@ -3107,10 +3107,10 @@
         <v>157710</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="25" t="s">
@@ -3132,7 +3132,7 @@
       <c r="N35" s="26"/>
       <c r="O35" s="26"/>
       <c r="P35" s="26" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="Q35" s="7"/>
       <c r="R35" s="7"/>
@@ -3147,10 +3147,10 @@
         <v>27024</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="25" t="s">
@@ -3170,7 +3170,7 @@
       <c r="N36" s="26"/>
       <c r="O36" s="26"/>
       <c r="P36" s="26" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="Q36" s="7"/>
       <c r="R36" s="7"/>
@@ -3185,10 +3185,10 @@
         <v>66790</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="25" t="s">
@@ -3210,7 +3210,7 @@
       <c r="N37" s="26"/>
       <c r="O37" s="26"/>
       <c r="P37" s="26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Q37" s="7"/>
       <c r="R37" s="7"/>
@@ -3219,16 +3219,16 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B38" s="16">
         <v>125838</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="25" t="s">
@@ -3248,7 +3248,7 @@
       <c r="N38" s="26"/>
       <c r="O38" s="26"/>
       <c r="P38" s="26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Q38" s="7"/>
       <c r="R38" s="7"/>
@@ -3263,10 +3263,10 @@
         <v>42464</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="25" t="s">
@@ -3286,7 +3286,7 @@
       <c r="N39" s="26"/>
       <c r="O39" s="26"/>
       <c r="P39" s="26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Q39" s="7"/>
       <c r="R39" s="7"/>
@@ -3301,10 +3301,10 @@
         <v>27026</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="25" t="s">
@@ -3326,7 +3326,7 @@
       <c r="N40" s="26"/>
       <c r="O40" s="26"/>
       <c r="P40" s="11" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="Q40" s="7"/>
       <c r="R40" s="7"/>
@@ -3341,10 +3341,10 @@
         <v>68304</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E41" s="28"/>
       <c r="F41" s="25" t="s">
@@ -3363,7 +3363,7 @@
       <c r="N41" s="30"/>
       <c r="O41" s="30"/>
       <c r="P41" s="11" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="Q41" s="28"/>
       <c r="R41" s="28"/>
@@ -3371,18 +3371,10 @@
       <c r="T41" s="31"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="P7" r:id="rId1" display="doe@example.com"/>
-    <hyperlink ref="P21" r:id="rId2" display="baby.doe@example.com"/>
-    <hyperlink ref="P23" r:id="rId3" display="doe@example.com"/>
-    <hyperlink ref="P8:P19" r:id="rId4" display="doe@example.com"/>
-    <hyperlink ref="P20" r:id="rId5" display="doe@example.com"/>
-    <hyperlink ref="P24:P34" r:id="rId6" display="doe@example.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3408,7 +3400,7 @@
     <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
@@ -3432,7 +3424,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>8</v>
@@ -3462,12 +3454,12 @@
         <v>56</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>3</v>
@@ -3479,7 +3471,7 @@
         <v>16</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -3496,16 +3488,16 @@
         <v>16</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>55</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>75</v>
@@ -3514,7 +3506,7 @@
         <v>73</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3540,7 +3532,7 @@
         <v>73</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3560,10 +3552,10 @@
         <v>0</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3589,7 +3581,7 @@
         <v>74</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="O6" s="14" t="s">
         <v>60</v>
@@ -3618,7 +3610,7 @@
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
@@ -3629,7 +3621,7 @@
         <v>157710</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>84</v>
@@ -3647,7 +3639,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="L8" s="14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
@@ -3658,7 +3650,7 @@
         <v>66790</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>84</v>
@@ -3676,7 +3668,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" s="14" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
@@ -3687,7 +3679,7 @@
         <v>27026</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>84</v>
@@ -3705,7 +3697,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" s="11" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>

</xml_diff>

<commit_message>
ISAICP-3862: Refactor 'case' documents file migration.
</commit_message>
<xml_diff>
--- a/resources/migrate/mapping-test.xlsx
+++ b/resources/migrate/mapping-test.xlsx
@@ -16,7 +16,7 @@
     <sheet name="5. Collections" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$T$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Content items'!$A$1:$T$44</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="120">
   <si>
     <t>No</t>
   </si>
@@ -385,6 +385,15 @@
   </si>
   <si>
     <t>user9351@example.com</t>
+  </si>
+  <si>
+    <t>General case study with files</t>
+  </si>
+  <si>
+    <t>Guideline with files</t>
+  </si>
+  <si>
+    <t>Open source case study with files</t>
   </si>
 </sst>
 </file>
@@ -612,7 +621,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="161">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -773,6 +782,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
@@ -871,7 +888,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="161">
+  <cellStyles count="169">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1009,6 +1026,10 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1031,6 +1052,10 @@
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="1"/>
   </cellStyles>
@@ -1370,8 +1395,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:T41" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:T41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table18915" displayName="Table18915" ref="A1:T44" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:T44"/>
   <sortState ref="A13187:X13200">
     <sortCondition ref="D2:D13200"/>
   </sortState>
@@ -1667,7 +1692,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:T41"/>
+  <dimension ref="A1:T44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3369,6 +3394,117 @@
       <c r="R41" s="28"/>
       <c r="S41" s="28"/>
       <c r="T41" s="31"/>
+    </row>
+    <row r="42" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="29">
+        <v>144018</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="29"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="30"/>
+      <c r="O42" s="30"/>
+      <c r="P42" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="31"/>
+    </row>
+    <row r="43" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="29">
+        <v>135110</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E43" s="28"/>
+      <c r="F43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="29"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="28"/>
+      <c r="N43" s="30"/>
+      <c r="O43" s="30"/>
+      <c r="P43" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q43" s="28"/>
+      <c r="R43" s="28"/>
+      <c r="S43" s="28"/>
+      <c r="T43" s="31"/>
+    </row>
+    <row r="44" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="29">
+        <v>135160</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="28"/>
+      <c r="F44" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="29"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="30"/>
+      <c r="O44" s="30"/>
+      <c r="P44" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q44" s="28"/>
+      <c r="R44" s="28"/>
+      <c r="S44" s="28"/>
+      <c r="T44" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>